<commit_message>
23 feb 2023 update
23 feb 2023 update dsr
</commit_message>
<xml_diff>
--- a/feb/feb2023.xlsx
+++ b/feb/feb2023.xlsx
@@ -111,9 +111,6 @@
     <t>WBX-4124</t>
   </si>
   <si>
-    <t xml:space="preserve">rebase the branch and update code push into git </t>
-  </si>
-  <si>
     <t>meeting with nidhi ma'am</t>
   </si>
   <si>
@@ -127,6 +124,9 @@
   </si>
   <si>
     <t>interuption of power cut N Change laptop again N install require softwares for project</t>
+  </si>
+  <si>
+    <t>rebase the branch and update code push into git N fix the issue</t>
   </si>
 </sst>
 </file>
@@ -424,21 +424,112 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="2" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -448,97 +539,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -1298,7 +1298,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1309,7 +1309,7 @@
   <dimension ref="A1:N181"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="O184" sqref="O184"/>
+      <selection activeCell="M190" sqref="M190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1325,18 +1325,18 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="49"/>
+      <c r="A3" s="35"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="49"/>
+      <c r="A4" s="35"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="49"/>
+      <c r="A5" s="35"/>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
@@ -1344,27 +1344,27 @@
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="35" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="49"/>
+      <c r="A11" s="35"/>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="49"/>
+      <c r="A12" s="35"/>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="49"/>
+      <c r="A13" s="35"/>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="49"/>
+      <c r="A14" s="35"/>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="49"/>
+      <c r="A15" s="35"/>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="49"/>
+      <c r="A16" s="35"/>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
@@ -1372,24 +1372,24 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="35" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="49"/>
+      <c r="A22" s="35"/>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="49"/>
+      <c r="A23" s="35"/>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="49"/>
+      <c r="A24" s="35"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="49"/>
+      <c r="A25" s="35"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="49"/>
+      <c r="A26" s="35"/>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="2"/>
@@ -1401,74 +1401,74 @@
       <c r="B29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="37"/>
-      <c r="L29" s="37"/>
-      <c r="M29" s="37"/>
-      <c r="N29" s="38"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="34"/>
     </row>
     <row r="30" spans="1:14">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="33">
+      <c r="B30" s="20">
         <v>44961</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="23"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="25"/>
     </row>
     <row r="31" spans="1:14">
-      <c r="A31" s="31"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="26"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="27"/>
+      <c r="N31" s="28"/>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="32"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="28"/>
-      <c r="M32" s="28"/>
-      <c r="N32" s="29"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="30"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="31"/>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="3" t="s">
@@ -1477,74 +1477,74 @@
       <c r="B35" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="37"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="37"/>
-      <c r="N35" s="38"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="33"/>
+      <c r="M35" s="33"/>
+      <c r="N35" s="34"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="33">
+      <c r="B36" s="20">
         <v>44962</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="23"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="24"/>
+      <c r="M36" s="24"/>
+      <c r="N36" s="25"/>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="31"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="25"/>
-      <c r="M37" s="25"/>
-      <c r="N37" s="26"/>
+      <c r="A37" s="18"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="27"/>
+      <c r="N37" s="28"/>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="32"/>
-      <c r="B38" s="35"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="28"/>
-      <c r="K38" s="28"/>
-      <c r="L38" s="28"/>
-      <c r="M38" s="28"/>
-      <c r="N38" s="29"/>
+      <c r="A38" s="19"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="30"/>
+      <c r="L38" s="30"/>
+      <c r="M38" s="30"/>
+      <c r="N38" s="31"/>
     </row>
     <row r="41" spans="1:14">
       <c r="A41" s="3" t="s">
@@ -1552,18 +1552,18 @@
       </c>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="14"/>
+      <c r="A43" s="15"/>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="14"/>
+      <c r="A44" s="15"/>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="14"/>
+      <c r="A45" s="15"/>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="3" t="s">
@@ -1571,15 +1571,15 @@
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="14"/>
+      <c r="A51" s="15"/>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="14"/>
+      <c r="A52" s="15"/>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="5" t="s">
@@ -1587,27 +1587,27 @@
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="39" t="s">
+      <c r="A56" s="36" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="39"/>
+      <c r="A57" s="36"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="39"/>
+      <c r="A58" s="36"/>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="39"/>
+      <c r="A59" s="36"/>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="39"/>
+      <c r="A60" s="36"/>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="39"/>
+      <c r="A61" s="36"/>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="39"/>
+      <c r="A62" s="36"/>
     </row>
     <row r="66" spans="1:14">
       <c r="A66" s="5" t="s">
@@ -1615,27 +1615,27 @@
       </c>
     </row>
     <row r="67" spans="1:14">
-      <c r="A67" s="39" t="s">
+      <c r="A67" s="36" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:14">
-      <c r="A68" s="39"/>
+      <c r="A68" s="36"/>
     </row>
     <row r="69" spans="1:14">
-      <c r="A69" s="39"/>
+      <c r="A69" s="36"/>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="39"/>
+      <c r="A70" s="36"/>
     </row>
     <row r="71" spans="1:14">
-      <c r="A71" s="39"/>
+      <c r="A71" s="36"/>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="39"/>
+      <c r="A72" s="36"/>
     </row>
     <row r="73" spans="1:14">
-      <c r="A73" s="39"/>
+      <c r="A73" s="36"/>
     </row>
     <row r="77" spans="1:14">
       <c r="A77" s="3" t="s">
@@ -1644,74 +1644,74 @@
       <c r="B77" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C77" s="36" t="s">
+      <c r="C77" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D77" s="37"/>
-      <c r="E77" s="37"/>
-      <c r="F77" s="37"/>
-      <c r="G77" s="37"/>
-      <c r="H77" s="37"/>
-      <c r="I77" s="37"/>
-      <c r="J77" s="37"/>
-      <c r="K77" s="37"/>
-      <c r="L77" s="37"/>
-      <c r="M77" s="37"/>
-      <c r="N77" s="38"/>
+      <c r="D77" s="33"/>
+      <c r="E77" s="33"/>
+      <c r="F77" s="33"/>
+      <c r="G77" s="33"/>
+      <c r="H77" s="33"/>
+      <c r="I77" s="33"/>
+      <c r="J77" s="33"/>
+      <c r="K77" s="33"/>
+      <c r="L77" s="33"/>
+      <c r="M77" s="33"/>
+      <c r="N77" s="34"/>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="30" t="s">
+      <c r="A78" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B78" s="33">
+      <c r="B78" s="20">
         <v>44967</v>
       </c>
-      <c r="C78" s="40" t="s">
+      <c r="C78" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="D78" s="41"/>
-      <c r="E78" s="41"/>
-      <c r="F78" s="41"/>
-      <c r="G78" s="41"/>
-      <c r="H78" s="41"/>
-      <c r="I78" s="41"/>
-      <c r="J78" s="41"/>
-      <c r="K78" s="41"/>
-      <c r="L78" s="41"/>
-      <c r="M78" s="41"/>
-      <c r="N78" s="42"/>
+      <c r="D78" s="38"/>
+      <c r="E78" s="38"/>
+      <c r="F78" s="38"/>
+      <c r="G78" s="38"/>
+      <c r="H78" s="38"/>
+      <c r="I78" s="38"/>
+      <c r="J78" s="38"/>
+      <c r="K78" s="38"/>
+      <c r="L78" s="38"/>
+      <c r="M78" s="38"/>
+      <c r="N78" s="39"/>
     </row>
     <row r="79" spans="1:14">
-      <c r="A79" s="31"/>
-      <c r="B79" s="34"/>
-      <c r="C79" s="43"/>
-      <c r="D79" s="44"/>
-      <c r="E79" s="44"/>
-      <c r="F79" s="44"/>
-      <c r="G79" s="44"/>
-      <c r="H79" s="44"/>
-      <c r="I79" s="44"/>
-      <c r="J79" s="44"/>
-      <c r="K79" s="44"/>
-      <c r="L79" s="44"/>
-      <c r="M79" s="44"/>
-      <c r="N79" s="45"/>
+      <c r="A79" s="18"/>
+      <c r="B79" s="21"/>
+      <c r="C79" s="40"/>
+      <c r="D79" s="41"/>
+      <c r="E79" s="41"/>
+      <c r="F79" s="41"/>
+      <c r="G79" s="41"/>
+      <c r="H79" s="41"/>
+      <c r="I79" s="41"/>
+      <c r="J79" s="41"/>
+      <c r="K79" s="41"/>
+      <c r="L79" s="41"/>
+      <c r="M79" s="41"/>
+      <c r="N79" s="42"/>
     </row>
     <row r="80" spans="1:14">
-      <c r="A80" s="32"/>
-      <c r="B80" s="35"/>
-      <c r="C80" s="46"/>
-      <c r="D80" s="47"/>
-      <c r="E80" s="47"/>
-      <c r="F80" s="47"/>
-      <c r="G80" s="47"/>
-      <c r="H80" s="47"/>
-      <c r="I80" s="47"/>
-      <c r="J80" s="47"/>
-      <c r="K80" s="47"/>
-      <c r="L80" s="47"/>
-      <c r="M80" s="47"/>
-      <c r="N80" s="48"/>
+      <c r="A80" s="19"/>
+      <c r="B80" s="22"/>
+      <c r="C80" s="43"/>
+      <c r="D80" s="44"/>
+      <c r="E80" s="44"/>
+      <c r="F80" s="44"/>
+      <c r="G80" s="44"/>
+      <c r="H80" s="44"/>
+      <c r="I80" s="44"/>
+      <c r="J80" s="44"/>
+      <c r="K80" s="44"/>
+      <c r="L80" s="44"/>
+      <c r="M80" s="44"/>
+      <c r="N80" s="45"/>
     </row>
     <row r="83" spans="1:14">
       <c r="A83" s="3" t="s">
@@ -1720,74 +1720,74 @@
       <c r="B83" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C83" s="36" t="s">
+      <c r="C83" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D83" s="37"/>
-      <c r="E83" s="37"/>
-      <c r="F83" s="37"/>
-      <c r="G83" s="37"/>
-      <c r="H83" s="37"/>
-      <c r="I83" s="37"/>
-      <c r="J83" s="37"/>
-      <c r="K83" s="37"/>
-      <c r="L83" s="37"/>
-      <c r="M83" s="37"/>
-      <c r="N83" s="38"/>
+      <c r="D83" s="33"/>
+      <c r="E83" s="33"/>
+      <c r="F83" s="33"/>
+      <c r="G83" s="33"/>
+      <c r="H83" s="33"/>
+      <c r="I83" s="33"/>
+      <c r="J83" s="33"/>
+      <c r="K83" s="33"/>
+      <c r="L83" s="33"/>
+      <c r="M83" s="33"/>
+      <c r="N83" s="34"/>
     </row>
     <row r="84" spans="1:14">
-      <c r="A84" s="30" t="s">
+      <c r="A84" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B84" s="33">
+      <c r="B84" s="20">
         <v>44968</v>
       </c>
-      <c r="C84" s="21" t="s">
+      <c r="C84" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D84" s="22"/>
-      <c r="E84" s="22"/>
-      <c r="F84" s="22"/>
-      <c r="G84" s="22"/>
-      <c r="H84" s="22"/>
-      <c r="I84" s="22"/>
-      <c r="J84" s="22"/>
-      <c r="K84" s="22"/>
-      <c r="L84" s="22"/>
-      <c r="M84" s="22"/>
-      <c r="N84" s="23"/>
+      <c r="D84" s="24"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="24"/>
+      <c r="H84" s="24"/>
+      <c r="I84" s="24"/>
+      <c r="J84" s="24"/>
+      <c r="K84" s="24"/>
+      <c r="L84" s="24"/>
+      <c r="M84" s="24"/>
+      <c r="N84" s="25"/>
     </row>
     <row r="85" spans="1:14">
-      <c r="A85" s="31"/>
-      <c r="B85" s="34"/>
-      <c r="C85" s="24"/>
-      <c r="D85" s="25"/>
-      <c r="E85" s="25"/>
-      <c r="F85" s="25"/>
-      <c r="G85" s="25"/>
-      <c r="H85" s="25"/>
-      <c r="I85" s="25"/>
-      <c r="J85" s="25"/>
-      <c r="K85" s="25"/>
-      <c r="L85" s="25"/>
-      <c r="M85" s="25"/>
-      <c r="N85" s="26"/>
+      <c r="A85" s="18"/>
+      <c r="B85" s="21"/>
+      <c r="C85" s="26"/>
+      <c r="D85" s="27"/>
+      <c r="E85" s="27"/>
+      <c r="F85" s="27"/>
+      <c r="G85" s="27"/>
+      <c r="H85" s="27"/>
+      <c r="I85" s="27"/>
+      <c r="J85" s="27"/>
+      <c r="K85" s="27"/>
+      <c r="L85" s="27"/>
+      <c r="M85" s="27"/>
+      <c r="N85" s="28"/>
     </row>
     <row r="86" spans="1:14">
-      <c r="A86" s="32"/>
-      <c r="B86" s="35"/>
-      <c r="C86" s="27"/>
-      <c r="D86" s="28"/>
-      <c r="E86" s="28"/>
-      <c r="F86" s="28"/>
-      <c r="G86" s="28"/>
-      <c r="H86" s="28"/>
-      <c r="I86" s="28"/>
-      <c r="J86" s="28"/>
-      <c r="K86" s="28"/>
-      <c r="L86" s="28"/>
-      <c r="M86" s="28"/>
-      <c r="N86" s="29"/>
+      <c r="A86" s="19"/>
+      <c r="B86" s="22"/>
+      <c r="C86" s="29"/>
+      <c r="D86" s="30"/>
+      <c r="E86" s="30"/>
+      <c r="F86" s="30"/>
+      <c r="G86" s="30"/>
+      <c r="H86" s="30"/>
+      <c r="I86" s="30"/>
+      <c r="J86" s="30"/>
+      <c r="K86" s="30"/>
+      <c r="L86" s="30"/>
+      <c r="M86" s="30"/>
+      <c r="N86" s="31"/>
     </row>
     <row r="89" spans="1:14">
       <c r="A89" s="3" t="s">
@@ -1796,74 +1796,74 @@
       <c r="B89" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C89" s="36" t="s">
+      <c r="C89" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D89" s="37"/>
-      <c r="E89" s="37"/>
-      <c r="F89" s="37"/>
-      <c r="G89" s="37"/>
-      <c r="H89" s="37"/>
-      <c r="I89" s="37"/>
-      <c r="J89" s="37"/>
-      <c r="K89" s="37"/>
-      <c r="L89" s="37"/>
-      <c r="M89" s="37"/>
-      <c r="N89" s="38"/>
+      <c r="D89" s="33"/>
+      <c r="E89" s="33"/>
+      <c r="F89" s="33"/>
+      <c r="G89" s="33"/>
+      <c r="H89" s="33"/>
+      <c r="I89" s="33"/>
+      <c r="J89" s="33"/>
+      <c r="K89" s="33"/>
+      <c r="L89" s="33"/>
+      <c r="M89" s="33"/>
+      <c r="N89" s="34"/>
     </row>
     <row r="90" spans="1:14">
-      <c r="A90" s="30" t="s">
+      <c r="A90" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B90" s="33">
+      <c r="B90" s="20">
         <v>44969</v>
       </c>
-      <c r="C90" s="21" t="s">
+      <c r="C90" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D90" s="22"/>
-      <c r="E90" s="22"/>
-      <c r="F90" s="22"/>
-      <c r="G90" s="22"/>
-      <c r="H90" s="22"/>
-      <c r="I90" s="22"/>
-      <c r="J90" s="22"/>
-      <c r="K90" s="22"/>
-      <c r="L90" s="22"/>
-      <c r="M90" s="22"/>
-      <c r="N90" s="23"/>
+      <c r="D90" s="24"/>
+      <c r="E90" s="24"/>
+      <c r="F90" s="24"/>
+      <c r="G90" s="24"/>
+      <c r="H90" s="24"/>
+      <c r="I90" s="24"/>
+      <c r="J90" s="24"/>
+      <c r="K90" s="24"/>
+      <c r="L90" s="24"/>
+      <c r="M90" s="24"/>
+      <c r="N90" s="25"/>
     </row>
     <row r="91" spans="1:14">
-      <c r="A91" s="31"/>
-      <c r="B91" s="34"/>
-      <c r="C91" s="24"/>
-      <c r="D91" s="25"/>
-      <c r="E91" s="25"/>
-      <c r="F91" s="25"/>
-      <c r="G91" s="25"/>
-      <c r="H91" s="25"/>
-      <c r="I91" s="25"/>
-      <c r="J91" s="25"/>
-      <c r="K91" s="25"/>
-      <c r="L91" s="25"/>
-      <c r="M91" s="25"/>
-      <c r="N91" s="26"/>
+      <c r="A91" s="18"/>
+      <c r="B91" s="21"/>
+      <c r="C91" s="26"/>
+      <c r="D91" s="27"/>
+      <c r="E91" s="27"/>
+      <c r="F91" s="27"/>
+      <c r="G91" s="27"/>
+      <c r="H91" s="27"/>
+      <c r="I91" s="27"/>
+      <c r="J91" s="27"/>
+      <c r="K91" s="27"/>
+      <c r="L91" s="27"/>
+      <c r="M91" s="27"/>
+      <c r="N91" s="28"/>
     </row>
     <row r="92" spans="1:14">
-      <c r="A92" s="32"/>
-      <c r="B92" s="35"/>
-      <c r="C92" s="27"/>
-      <c r="D92" s="28"/>
-      <c r="E92" s="28"/>
-      <c r="F92" s="28"/>
-      <c r="G92" s="28"/>
-      <c r="H92" s="28"/>
-      <c r="I92" s="28"/>
-      <c r="J92" s="28"/>
-      <c r="K92" s="28"/>
-      <c r="L92" s="28"/>
-      <c r="M92" s="28"/>
-      <c r="N92" s="29"/>
+      <c r="A92" s="19"/>
+      <c r="B92" s="22"/>
+      <c r="C92" s="29"/>
+      <c r="D92" s="30"/>
+      <c r="E92" s="30"/>
+      <c r="F92" s="30"/>
+      <c r="G92" s="30"/>
+      <c r="H92" s="30"/>
+      <c r="I92" s="30"/>
+      <c r="J92" s="30"/>
+      <c r="K92" s="30"/>
+      <c r="L92" s="30"/>
+      <c r="M92" s="30"/>
+      <c r="N92" s="31"/>
     </row>
     <row r="144" spans="1:14">
       <c r="A144" s="3" t="s">
@@ -1888,58 +1888,58 @@
       <c r="N144" s="8"/>
     </row>
     <row r="145" spans="1:14">
-      <c r="A145" s="30" t="s">
+      <c r="A145" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B145" s="33">
+      <c r="B145" s="20">
         <v>44975</v>
       </c>
-      <c r="C145" s="21" t="s">
+      <c r="C145" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D145" s="22"/>
-      <c r="E145" s="22"/>
-      <c r="F145" s="22"/>
-      <c r="G145" s="22"/>
-      <c r="H145" s="22"/>
-      <c r="I145" s="22"/>
-      <c r="J145" s="22"/>
-      <c r="K145" s="22"/>
-      <c r="L145" s="22"/>
-      <c r="M145" s="22"/>
-      <c r="N145" s="23"/>
+      <c r="D145" s="24"/>
+      <c r="E145" s="24"/>
+      <c r="F145" s="24"/>
+      <c r="G145" s="24"/>
+      <c r="H145" s="24"/>
+      <c r="I145" s="24"/>
+      <c r="J145" s="24"/>
+      <c r="K145" s="24"/>
+      <c r="L145" s="24"/>
+      <c r="M145" s="24"/>
+      <c r="N145" s="25"/>
     </row>
     <row r="146" spans="1:14">
-      <c r="A146" s="31"/>
-      <c r="B146" s="34"/>
-      <c r="C146" s="24"/>
-      <c r="D146" s="25"/>
-      <c r="E146" s="25"/>
-      <c r="F146" s="25"/>
-      <c r="G146" s="25"/>
-      <c r="H146" s="25"/>
-      <c r="I146" s="25"/>
-      <c r="J146" s="25"/>
-      <c r="K146" s="25"/>
-      <c r="L146" s="25"/>
-      <c r="M146" s="25"/>
-      <c r="N146" s="26"/>
+      <c r="A146" s="18"/>
+      <c r="B146" s="21"/>
+      <c r="C146" s="26"/>
+      <c r="D146" s="27"/>
+      <c r="E146" s="27"/>
+      <c r="F146" s="27"/>
+      <c r="G146" s="27"/>
+      <c r="H146" s="27"/>
+      <c r="I146" s="27"/>
+      <c r="J146" s="27"/>
+      <c r="K146" s="27"/>
+      <c r="L146" s="27"/>
+      <c r="M146" s="27"/>
+      <c r="N146" s="28"/>
     </row>
     <row r="147" spans="1:14">
-      <c r="A147" s="32"/>
-      <c r="B147" s="35"/>
-      <c r="C147" s="27"/>
-      <c r="D147" s="28"/>
-      <c r="E147" s="28"/>
-      <c r="F147" s="28"/>
-      <c r="G147" s="28"/>
-      <c r="H147" s="28"/>
-      <c r="I147" s="28"/>
-      <c r="J147" s="28"/>
-      <c r="K147" s="28"/>
-      <c r="L147" s="28"/>
-      <c r="M147" s="28"/>
-      <c r="N147" s="29"/>
+      <c r="A147" s="19"/>
+      <c r="B147" s="22"/>
+      <c r="C147" s="29"/>
+      <c r="D147" s="30"/>
+      <c r="E147" s="30"/>
+      <c r="F147" s="30"/>
+      <c r="G147" s="30"/>
+      <c r="H147" s="30"/>
+      <c r="I147" s="30"/>
+      <c r="J147" s="30"/>
+      <c r="K147" s="30"/>
+      <c r="L147" s="30"/>
+      <c r="M147" s="30"/>
+      <c r="N147" s="31"/>
     </row>
     <row r="150" spans="1:14">
       <c r="A150" s="3" t="s">
@@ -1964,58 +1964,58 @@
       <c r="N150" s="8"/>
     </row>
     <row r="151" spans="1:14">
-      <c r="A151" s="30" t="s">
+      <c r="A151" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B151" s="33">
+      <c r="B151" s="20">
         <v>44976</v>
       </c>
-      <c r="C151" s="21" t="s">
+      <c r="C151" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D151" s="22"/>
-      <c r="E151" s="22"/>
-      <c r="F151" s="22"/>
-      <c r="G151" s="22"/>
-      <c r="H151" s="22"/>
-      <c r="I151" s="22"/>
-      <c r="J151" s="22"/>
-      <c r="K151" s="22"/>
-      <c r="L151" s="22"/>
-      <c r="M151" s="22"/>
-      <c r="N151" s="23"/>
+      <c r="D151" s="24"/>
+      <c r="E151" s="24"/>
+      <c r="F151" s="24"/>
+      <c r="G151" s="24"/>
+      <c r="H151" s="24"/>
+      <c r="I151" s="24"/>
+      <c r="J151" s="24"/>
+      <c r="K151" s="24"/>
+      <c r="L151" s="24"/>
+      <c r="M151" s="24"/>
+      <c r="N151" s="25"/>
     </row>
     <row r="152" spans="1:14">
-      <c r="A152" s="31"/>
-      <c r="B152" s="34"/>
-      <c r="C152" s="24"/>
-      <c r="D152" s="25"/>
-      <c r="E152" s="25"/>
-      <c r="F152" s="25"/>
-      <c r="G152" s="25"/>
-      <c r="H152" s="25"/>
-      <c r="I152" s="25"/>
-      <c r="J152" s="25"/>
-      <c r="K152" s="25"/>
-      <c r="L152" s="25"/>
-      <c r="M152" s="25"/>
-      <c r="N152" s="26"/>
+      <c r="A152" s="18"/>
+      <c r="B152" s="21"/>
+      <c r="C152" s="26"/>
+      <c r="D152" s="27"/>
+      <c r="E152" s="27"/>
+      <c r="F152" s="27"/>
+      <c r="G152" s="27"/>
+      <c r="H152" s="27"/>
+      <c r="I152" s="27"/>
+      <c r="J152" s="27"/>
+      <c r="K152" s="27"/>
+      <c r="L152" s="27"/>
+      <c r="M152" s="27"/>
+      <c r="N152" s="28"/>
     </row>
     <row r="153" spans="1:14">
-      <c r="A153" s="32"/>
-      <c r="B153" s="35"/>
-      <c r="C153" s="27"/>
-      <c r="D153" s="28"/>
-      <c r="E153" s="28"/>
-      <c r="F153" s="28"/>
-      <c r="G153" s="28"/>
-      <c r="H153" s="28"/>
-      <c r="I153" s="28"/>
-      <c r="J153" s="28"/>
-      <c r="K153" s="28"/>
-      <c r="L153" s="28"/>
-      <c r="M153" s="28"/>
-      <c r="N153" s="29"/>
+      <c r="A153" s="19"/>
+      <c r="B153" s="22"/>
+      <c r="C153" s="29"/>
+      <c r="D153" s="30"/>
+      <c r="E153" s="30"/>
+      <c r="F153" s="30"/>
+      <c r="G153" s="30"/>
+      <c r="H153" s="30"/>
+      <c r="I153" s="30"/>
+      <c r="J153" s="30"/>
+      <c r="K153" s="30"/>
+      <c r="L153" s="30"/>
+      <c r="M153" s="30"/>
+      <c r="N153" s="31"/>
     </row>
     <row r="156" spans="1:14">
       <c r="A156" s="3" t="s">
@@ -2033,23 +2033,23 @@
       <c r="E156" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F156" s="12" t="s">
+      <c r="F156" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="G156" s="13"/>
-      <c r="H156" s="13"/>
-      <c r="I156" s="13"/>
-      <c r="J156" s="13"/>
-      <c r="K156" s="13"/>
-      <c r="L156" s="13"/>
-      <c r="M156" s="13"/>
-      <c r="N156" s="13"/>
+      <c r="G156" s="47"/>
+      <c r="H156" s="47"/>
+      <c r="I156" s="47"/>
+      <c r="J156" s="47"/>
+      <c r="K156" s="47"/>
+      <c r="L156" s="47"/>
+      <c r="M156" s="47"/>
+      <c r="N156" s="47"/>
     </row>
     <row r="157" spans="1:14">
-      <c r="A157" s="14" t="s">
+      <c r="A157" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B157" s="15">
+      <c r="B157" s="16">
         <v>44977</v>
       </c>
       <c r="C157" s="9" t="s">
@@ -2061,21 +2061,21 @@
       <c r="E157" s="9">
         <v>0.40277777777777773</v>
       </c>
-      <c r="F157" s="16" t="s">
+      <c r="F157" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G157" s="16"/>
-      <c r="H157" s="16"/>
-      <c r="I157" s="16"/>
-      <c r="J157" s="16"/>
-      <c r="K157" s="16"/>
-      <c r="L157" s="16"/>
-      <c r="M157" s="16"/>
-      <c r="N157" s="16"/>
+      <c r="G157" s="13"/>
+      <c r="H157" s="13"/>
+      <c r="I157" s="13"/>
+      <c r="J157" s="13"/>
+      <c r="K157" s="13"/>
+      <c r="L157" s="13"/>
+      <c r="M157" s="13"/>
+      <c r="N157" s="13"/>
     </row>
     <row r="158" spans="1:14">
-      <c r="A158" s="14"/>
-      <c r="B158" s="15"/>
+      <c r="A158" s="15"/>
+      <c r="B158" s="16"/>
       <c r="C158" s="9" t="s">
         <v>19</v>
       </c>
@@ -2085,21 +2085,21 @@
       <c r="E158" s="9">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F158" s="16" t="s">
+      <c r="F158" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G158" s="16"/>
-      <c r="H158" s="16"/>
-      <c r="I158" s="16"/>
-      <c r="J158" s="16"/>
-      <c r="K158" s="16"/>
-      <c r="L158" s="16"/>
-      <c r="M158" s="16"/>
-      <c r="N158" s="16"/>
+      <c r="G158" s="13"/>
+      <c r="H158" s="13"/>
+      <c r="I158" s="13"/>
+      <c r="J158" s="13"/>
+      <c r="K158" s="13"/>
+      <c r="L158" s="13"/>
+      <c r="M158" s="13"/>
+      <c r="N158" s="13"/>
     </row>
     <row r="159" spans="1:14">
-      <c r="A159" s="14"/>
-      <c r="B159" s="15"/>
+      <c r="A159" s="15"/>
+      <c r="B159" s="16"/>
       <c r="C159" s="10" t="s">
         <v>21</v>
       </c>
@@ -2109,21 +2109,21 @@
       <c r="E159" s="9">
         <v>0.22916666666666666</v>
       </c>
-      <c r="F159" s="17" t="s">
+      <c r="F159" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="G159" s="18"/>
-      <c r="H159" s="18"/>
-      <c r="I159" s="18"/>
-      <c r="J159" s="18"/>
-      <c r="K159" s="18"/>
-      <c r="L159" s="18"/>
-      <c r="M159" s="18"/>
-      <c r="N159" s="19"/>
+      <c r="G159" s="49"/>
+      <c r="H159" s="49"/>
+      <c r="I159" s="49"/>
+      <c r="J159" s="49"/>
+      <c r="K159" s="49"/>
+      <c r="L159" s="49"/>
+      <c r="M159" s="49"/>
+      <c r="N159" s="50"/>
     </row>
     <row r="160" spans="1:14">
-      <c r="A160" s="14"/>
-      <c r="B160" s="15"/>
+      <c r="A160" s="15"/>
+      <c r="B160" s="16"/>
       <c r="C160" s="10" t="s">
         <v>23</v>
       </c>
@@ -2133,17 +2133,17 @@
       <c r="E160" s="9">
         <v>0.27083333333333331</v>
       </c>
-      <c r="F160" s="16" t="s">
+      <c r="F160" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G160" s="16"/>
-      <c r="H160" s="16"/>
-      <c r="I160" s="16"/>
-      <c r="J160" s="16"/>
-      <c r="K160" s="16"/>
-      <c r="L160" s="16"/>
-      <c r="M160" s="16"/>
-      <c r="N160" s="16"/>
+      <c r="G160" s="13"/>
+      <c r="H160" s="13"/>
+      <c r="I160" s="13"/>
+      <c r="J160" s="13"/>
+      <c r="K160" s="13"/>
+      <c r="L160" s="13"/>
+      <c r="M160" s="13"/>
+      <c r="N160" s="13"/>
     </row>
     <row r="163" spans="1:14">
       <c r="A163" s="3" t="s">
@@ -2161,23 +2161,23 @@
       <c r="E163" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F163" s="20" t="s">
+      <c r="F163" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G163" s="20"/>
-      <c r="H163" s="20"/>
-      <c r="I163" s="20"/>
-      <c r="J163" s="20"/>
-      <c r="K163" s="20"/>
-      <c r="L163" s="20"/>
-      <c r="M163" s="20"/>
-      <c r="N163" s="20"/>
+      <c r="G163" s="14"/>
+      <c r="H163" s="14"/>
+      <c r="I163" s="14"/>
+      <c r="J163" s="14"/>
+      <c r="K163" s="14"/>
+      <c r="L163" s="14"/>
+      <c r="M163" s="14"/>
+      <c r="N163" s="14"/>
     </row>
     <row r="164" spans="1:14">
-      <c r="A164" s="14" t="s">
+      <c r="A164" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B164" s="15">
+      <c r="B164" s="16">
         <v>44978</v>
       </c>
       <c r="C164" s="9" t="s">
@@ -2189,21 +2189,21 @@
       <c r="E164" s="9">
         <v>0.40277777777777773</v>
       </c>
-      <c r="F164" s="16" t="s">
+      <c r="F164" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G164" s="16"/>
-      <c r="H164" s="16"/>
-      <c r="I164" s="16"/>
-      <c r="J164" s="16"/>
-      <c r="K164" s="16"/>
-      <c r="L164" s="16"/>
-      <c r="M164" s="16"/>
-      <c r="N164" s="16"/>
+      <c r="G164" s="13"/>
+      <c r="H164" s="13"/>
+      <c r="I164" s="13"/>
+      <c r="J164" s="13"/>
+      <c r="K164" s="13"/>
+      <c r="L164" s="13"/>
+      <c r="M164" s="13"/>
+      <c r="N164" s="13"/>
     </row>
     <row r="165" spans="1:14">
-      <c r="A165" s="14"/>
-      <c r="B165" s="15"/>
+      <c r="A165" s="15"/>
+      <c r="B165" s="16"/>
       <c r="C165" s="10" t="s">
         <v>12</v>
       </c>
@@ -2213,21 +2213,21 @@
       <c r="E165" s="9">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F165" s="16" t="s">
+      <c r="F165" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G165" s="16"/>
-      <c r="H165" s="16"/>
-      <c r="I165" s="16"/>
-      <c r="J165" s="16"/>
-      <c r="K165" s="16"/>
-      <c r="L165" s="16"/>
-      <c r="M165" s="16"/>
-      <c r="N165" s="16"/>
+      <c r="G165" s="13"/>
+      <c r="H165" s="13"/>
+      <c r="I165" s="13"/>
+      <c r="J165" s="13"/>
+      <c r="K165" s="13"/>
+      <c r="L165" s="13"/>
+      <c r="M165" s="13"/>
+      <c r="N165" s="13"/>
     </row>
     <row r="166" spans="1:14">
-      <c r="A166" s="14"/>
-      <c r="B166" s="15"/>
+      <c r="A166" s="15"/>
+      <c r="B166" s="16"/>
       <c r="C166" s="10" t="s">
         <v>12</v>
       </c>
@@ -2237,17 +2237,17 @@
       <c r="E166" s="9">
         <v>0.27083333333333331</v>
       </c>
-      <c r="F166" s="16" t="s">
+      <c r="F166" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G166" s="16"/>
-      <c r="H166" s="16"/>
-      <c r="I166" s="16"/>
-      <c r="J166" s="16"/>
-      <c r="K166" s="16"/>
-      <c r="L166" s="16"/>
-      <c r="M166" s="16"/>
-      <c r="N166" s="16"/>
+      <c r="G166" s="13"/>
+      <c r="H166" s="13"/>
+      <c r="I166" s="13"/>
+      <c r="J166" s="13"/>
+      <c r="K166" s="13"/>
+      <c r="L166" s="13"/>
+      <c r="M166" s="13"/>
+      <c r="N166" s="13"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="4" t="s">
@@ -2265,23 +2265,23 @@
       <c r="E169" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F169" s="20" t="s">
+      <c r="F169" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G169" s="20"/>
-      <c r="H169" s="20"/>
-      <c r="I169" s="20"/>
-      <c r="J169" s="20"/>
-      <c r="K169" s="20"/>
-      <c r="L169" s="20"/>
-      <c r="M169" s="20"/>
-      <c r="N169" s="20"/>
+      <c r="G169" s="14"/>
+      <c r="H169" s="14"/>
+      <c r="I169" s="14"/>
+      <c r="J169" s="14"/>
+      <c r="K169" s="14"/>
+      <c r="L169" s="14"/>
+      <c r="M169" s="14"/>
+      <c r="N169" s="14"/>
     </row>
     <row r="170" spans="1:14">
-      <c r="A170" s="14" t="s">
+      <c r="A170" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B170" s="15">
+      <c r="B170" s="16">
         <v>44979</v>
       </c>
       <c r="C170" s="9" t="s">
@@ -2293,21 +2293,21 @@
       <c r="E170" s="9">
         <v>0.40277777777777773</v>
       </c>
-      <c r="F170" s="16" t="s">
+      <c r="F170" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G170" s="16"/>
-      <c r="H170" s="16"/>
-      <c r="I170" s="16"/>
-      <c r="J170" s="16"/>
-      <c r="K170" s="16"/>
-      <c r="L170" s="16"/>
-      <c r="M170" s="16"/>
-      <c r="N170" s="16"/>
+      <c r="G170" s="13"/>
+      <c r="H170" s="13"/>
+      <c r="I170" s="13"/>
+      <c r="J170" s="13"/>
+      <c r="K170" s="13"/>
+      <c r="L170" s="13"/>
+      <c r="M170" s="13"/>
+      <c r="N170" s="13"/>
     </row>
     <row r="171" spans="1:14">
-      <c r="A171" s="14"/>
-      <c r="B171" s="15"/>
+      <c r="A171" s="15"/>
+      <c r="B171" s="16"/>
       <c r="C171" s="10" t="s">
         <v>21</v>
       </c>
@@ -2317,21 +2317,21 @@
       <c r="E171" s="9">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F171" s="16" t="s">
+      <c r="F171" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="G171" s="16"/>
-      <c r="H171" s="16"/>
-      <c r="I171" s="16"/>
-      <c r="J171" s="16"/>
-      <c r="K171" s="16"/>
-      <c r="L171" s="16"/>
-      <c r="M171" s="16"/>
-      <c r="N171" s="16"/>
+      <c r="G171" s="13"/>
+      <c r="H171" s="13"/>
+      <c r="I171" s="13"/>
+      <c r="J171" s="13"/>
+      <c r="K171" s="13"/>
+      <c r="L171" s="13"/>
+      <c r="M171" s="13"/>
+      <c r="N171" s="13"/>
     </row>
     <row r="172" spans="1:14">
-      <c r="A172" s="14"/>
-      <c r="B172" s="15"/>
+      <c r="A172" s="15"/>
+      <c r="B172" s="16"/>
       <c r="C172" s="10" t="s">
         <v>12</v>
       </c>
@@ -2341,17 +2341,17 @@
       <c r="E172" s="9">
         <v>0.27083333333333331</v>
       </c>
-      <c r="F172" s="16" t="s">
+      <c r="F172" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G172" s="16"/>
-      <c r="H172" s="16"/>
-      <c r="I172" s="16"/>
-      <c r="J172" s="16"/>
-      <c r="K172" s="16"/>
-      <c r="L172" s="16"/>
-      <c r="M172" s="16"/>
-      <c r="N172" s="16"/>
+      <c r="G172" s="13"/>
+      <c r="H172" s="13"/>
+      <c r="I172" s="13"/>
+      <c r="J172" s="13"/>
+      <c r="K172" s="13"/>
+      <c r="L172" s="13"/>
+      <c r="M172" s="13"/>
+      <c r="N172" s="13"/>
     </row>
     <row r="175" spans="1:14">
       <c r="A175" s="11" t="s">
@@ -2369,26 +2369,26 @@
       <c r="E175" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F175" s="20" t="s">
+      <c r="F175" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G175" s="20"/>
-      <c r="H175" s="20"/>
-      <c r="I175" s="20"/>
-      <c r="J175" s="20"/>
-      <c r="K175" s="20"/>
-      <c r="L175" s="20"/>
-      <c r="M175" s="20"/>
-      <c r="N175" s="20"/>
+      <c r="G175" s="14"/>
+      <c r="H175" s="14"/>
+      <c r="I175" s="14"/>
+      <c r="J175" s="14"/>
+      <c r="K175" s="14"/>
+      <c r="L175" s="14"/>
+      <c r="M175" s="14"/>
+      <c r="N175" s="14"/>
     </row>
     <row r="176" spans="1:14">
-      <c r="A176" s="14" t="s">
+      <c r="A176" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B176" s="15">
+      <c r="B176" s="16">
         <v>44980</v>
       </c>
-      <c r="C176" s="50" t="s">
+      <c r="C176" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D176" s="9">
@@ -2397,22 +2397,22 @@
       <c r="E176" s="9">
         <v>0.40277777777777773</v>
       </c>
-      <c r="F176" s="16" t="s">
+      <c r="F176" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G176" s="16"/>
-      <c r="H176" s="16"/>
-      <c r="I176" s="16"/>
-      <c r="J176" s="16"/>
-      <c r="K176" s="16"/>
-      <c r="L176" s="16"/>
-      <c r="M176" s="16"/>
-      <c r="N176" s="16"/>
+      <c r="G176" s="13"/>
+      <c r="H176" s="13"/>
+      <c r="I176" s="13"/>
+      <c r="J176" s="13"/>
+      <c r="K176" s="13"/>
+      <c r="L176" s="13"/>
+      <c r="M176" s="13"/>
+      <c r="N176" s="13"/>
     </row>
     <row r="177" spans="1:14">
-      <c r="A177" s="14"/>
-      <c r="B177" s="15"/>
-      <c r="C177" s="50" t="s">
+      <c r="A177" s="15"/>
+      <c r="B177" s="16"/>
+      <c r="C177" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D177" s="9">
@@ -2421,22 +2421,22 @@
       <c r="E177" s="9">
         <v>0.48125000000000001</v>
       </c>
-      <c r="F177" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G177" s="16"/>
-      <c r="H177" s="16"/>
-      <c r="I177" s="16"/>
-      <c r="J177" s="16"/>
-      <c r="K177" s="16"/>
-      <c r="L177" s="16"/>
-      <c r="M177" s="16"/>
-      <c r="N177" s="16"/>
+      <c r="F177" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G177" s="13"/>
+      <c r="H177" s="13"/>
+      <c r="I177" s="13"/>
+      <c r="J177" s="13"/>
+      <c r="K177" s="13"/>
+      <c r="L177" s="13"/>
+      <c r="M177" s="13"/>
+      <c r="N177" s="13"/>
     </row>
     <row r="178" spans="1:14">
-      <c r="A178" s="14"/>
-      <c r="B178" s="15"/>
-      <c r="C178" s="50" t="s">
+      <c r="A178" s="15"/>
+      <c r="B178" s="16"/>
+      <c r="C178" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D178" s="9">
@@ -2445,22 +2445,22 @@
       <c r="E178" s="9">
         <v>0.5</v>
       </c>
-      <c r="F178" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G178" s="16"/>
-      <c r="H178" s="16"/>
-      <c r="I178" s="16"/>
-      <c r="J178" s="16"/>
-      <c r="K178" s="16"/>
-      <c r="L178" s="16"/>
-      <c r="M178" s="16"/>
-      <c r="N178" s="16"/>
+      <c r="F178" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G178" s="13"/>
+      <c r="H178" s="13"/>
+      <c r="I178" s="13"/>
+      <c r="J178" s="13"/>
+      <c r="K178" s="13"/>
+      <c r="L178" s="13"/>
+      <c r="M178" s="13"/>
+      <c r="N178" s="13"/>
     </row>
     <row r="179" spans="1:14">
-      <c r="A179" s="14"/>
-      <c r="B179" s="15"/>
-      <c r="C179" s="50" t="s">
+      <c r="A179" s="15"/>
+      <c r="B179" s="16"/>
+      <c r="C179" s="12" t="s">
         <v>28</v>
       </c>
       <c r="D179" s="9">
@@ -2469,22 +2469,22 @@
       <c r="E179" s="9">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F179" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G179" s="16"/>
-      <c r="H179" s="16"/>
-      <c r="I179" s="16"/>
-      <c r="J179" s="16"/>
-      <c r="K179" s="16"/>
-      <c r="L179" s="16"/>
-      <c r="M179" s="16"/>
-      <c r="N179" s="16"/>
+      <c r="F179" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G179" s="13"/>
+      <c r="H179" s="13"/>
+      <c r="I179" s="13"/>
+      <c r="J179" s="13"/>
+      <c r="K179" s="13"/>
+      <c r="L179" s="13"/>
+      <c r="M179" s="13"/>
+      <c r="N179" s="13"/>
     </row>
     <row r="180" spans="1:14">
-      <c r="A180" s="14"/>
-      <c r="B180" s="15"/>
-      <c r="C180" s="50" t="s">
+      <c r="A180" s="15"/>
+      <c r="B180" s="16"/>
+      <c r="C180" s="12" t="s">
         <v>29</v>
       </c>
       <c r="D180" s="9">
@@ -2493,23 +2493,23 @@
       <c r="E180" s="9">
         <v>0.125</v>
       </c>
-      <c r="F180" s="16" t="s">
+      <c r="F180" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G180" s="13"/>
+      <c r="H180" s="13"/>
+      <c r="I180" s="13"/>
+      <c r="J180" s="13"/>
+      <c r="K180" s="13"/>
+      <c r="L180" s="13"/>
+      <c r="M180" s="13"/>
+      <c r="N180" s="13"/>
+    </row>
+    <row r="181" spans="1:14">
+      <c r="A181" s="15"/>
+      <c r="B181" s="16"/>
+      <c r="C181" s="12" t="s">
         <v>33</v>
-      </c>
-      <c r="G180" s="16"/>
-      <c r="H180" s="16"/>
-      <c r="I180" s="16"/>
-      <c r="J180" s="16"/>
-      <c r="K180" s="16"/>
-      <c r="L180" s="16"/>
-      <c r="M180" s="16"/>
-      <c r="N180" s="16"/>
-    </row>
-    <row r="181" spans="1:14">
-      <c r="A181" s="14"/>
-      <c r="B181" s="15"/>
-      <c r="C181" s="50" t="s">
-        <v>34</v>
       </c>
       <c r="D181" s="9">
         <v>0.125</v>
@@ -2517,20 +2517,66 @@
       <c r="E181" s="9">
         <v>0.27083333333333331</v>
       </c>
-      <c r="F181" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="G181" s="16"/>
-      <c r="H181" s="16"/>
-      <c r="I181" s="16"/>
-      <c r="J181" s="16"/>
-      <c r="K181" s="16"/>
-      <c r="L181" s="16"/>
-      <c r="M181" s="16"/>
-      <c r="N181" s="16"/>
+      <c r="F181" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G181" s="13"/>
+      <c r="H181" s="13"/>
+      <c r="I181" s="13"/>
+      <c r="J181" s="13"/>
+      <c r="K181" s="13"/>
+      <c r="L181" s="13"/>
+      <c r="M181" s="13"/>
+      <c r="N181" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="F156:N156"/>
+    <mergeCell ref="A157:A160"/>
+    <mergeCell ref="B157:B160"/>
+    <mergeCell ref="F157:N157"/>
+    <mergeCell ref="F158:N158"/>
+    <mergeCell ref="F159:N159"/>
+    <mergeCell ref="F160:N160"/>
+    <mergeCell ref="F163:N163"/>
+    <mergeCell ref="A164:A166"/>
+    <mergeCell ref="B164:B166"/>
+    <mergeCell ref="F164:N164"/>
+    <mergeCell ref="F165:N165"/>
+    <mergeCell ref="F166:N166"/>
+    <mergeCell ref="C145:N147"/>
+    <mergeCell ref="A151:A153"/>
+    <mergeCell ref="B151:B153"/>
+    <mergeCell ref="C151:N153"/>
+    <mergeCell ref="C90:N92"/>
+    <mergeCell ref="A90:A92"/>
+    <mergeCell ref="B90:B92"/>
+    <mergeCell ref="A145:A147"/>
+    <mergeCell ref="B145:B147"/>
+    <mergeCell ref="C89:N89"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="C84:N86"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A67:A73"/>
+    <mergeCell ref="C77:N77"/>
+    <mergeCell ref="A78:A80"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="C78:N80"/>
+    <mergeCell ref="C83:N83"/>
+    <mergeCell ref="C35:N35"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:N38"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:N32"/>
+    <mergeCell ref="C29:N29"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="A21:A26"/>
     <mergeCell ref="F181:N181"/>
     <mergeCell ref="F179:N179"/>
     <mergeCell ref="F180:N180"/>
@@ -2546,52 +2592,6 @@
     <mergeCell ref="F178:N178"/>
     <mergeCell ref="A176:A181"/>
     <mergeCell ref="B176:B181"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:N32"/>
-    <mergeCell ref="C29:N29"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A10:A16"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="C35:N35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C36:N38"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="C89:N89"/>
-    <mergeCell ref="A84:A86"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="C84:N86"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A67:A73"/>
-    <mergeCell ref="C77:N77"/>
-    <mergeCell ref="A78:A80"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="C78:N80"/>
-    <mergeCell ref="C83:N83"/>
-    <mergeCell ref="C145:N147"/>
-    <mergeCell ref="A151:A153"/>
-    <mergeCell ref="B151:B153"/>
-    <mergeCell ref="C151:N153"/>
-    <mergeCell ref="C90:N92"/>
-    <mergeCell ref="A90:A92"/>
-    <mergeCell ref="B90:B92"/>
-    <mergeCell ref="A145:A147"/>
-    <mergeCell ref="B145:B147"/>
-    <mergeCell ref="F163:N163"/>
-    <mergeCell ref="A164:A166"/>
-    <mergeCell ref="B164:B166"/>
-    <mergeCell ref="F164:N164"/>
-    <mergeCell ref="F165:N165"/>
-    <mergeCell ref="F166:N166"/>
-    <mergeCell ref="F156:N156"/>
-    <mergeCell ref="A157:A160"/>
-    <mergeCell ref="B157:B160"/>
-    <mergeCell ref="F157:N157"/>
-    <mergeCell ref="F158:N158"/>
-    <mergeCell ref="F159:N159"/>
-    <mergeCell ref="F160:N160"/>
   </mergeCells>
   <conditionalFormatting sqref="B90:C90">
     <cfRule type="timePeriod" dxfId="1" priority="2" timePeriod="lastMonth">

</xml_diff>

<commit_message>
24 feb 2023 dsr
24 feb 2023 dsr
</commit_message>
<xml_diff>
--- a/feb/feb2023.xlsx
+++ b/feb/feb2023.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="46">
   <si>
     <t>Day</t>
   </si>
@@ -127,6 +127,36 @@
   </si>
   <si>
     <t>rebase the branch and update code push into git N fix the issue</t>
+  </si>
+  <si>
+    <t>Raise the PR of browser tracket list</t>
+  </si>
+  <si>
+    <t>install node module for api-server N client directory N login git credential when code push</t>
+  </si>
+  <si>
+    <t>WBX-4123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raise the PR of browser tracket list when edit mode </t>
+  </si>
+  <si>
+    <t>WBX-3966</t>
+  </si>
+  <si>
+    <t>work on the login message showing at the same  time</t>
+  </si>
+  <si>
+    <t>WBX-4102</t>
+  </si>
+  <si>
+    <t>add the underscore regex in the password and raise the PR</t>
+  </si>
+  <si>
+    <t>WBX-4184</t>
+  </si>
+  <si>
+    <t>user module automatically fill username and Password and raise the PR</t>
   </si>
 </sst>
 </file>
@@ -393,7 +423,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -409,15 +439,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -425,16 +446,61 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -455,33 +521,6 @@
     <xf numFmtId="15" fontId="2" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -491,53 +530,47 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -548,7 +581,17 @@
     <cellStyle name="Bad" xfId="5" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1298,7 +1341,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1306,10 +1349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N181"/>
+  <dimension ref="A1:N206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="M190" sqref="M190"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="T195" sqref="T195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1325,18 +1368,18 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="48" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="35"/>
+      <c r="A3" s="48"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="35"/>
+      <c r="A4" s="48"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="35"/>
+      <c r="A5" s="48"/>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
@@ -1344,27 +1387,27 @@
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="48" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="35"/>
+      <c r="A11" s="48"/>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="35"/>
+      <c r="A12" s="48"/>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="35"/>
+      <c r="A13" s="48"/>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="35"/>
+      <c r="A14" s="48"/>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="35"/>
+      <c r="A15" s="48"/>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="35"/>
+      <c r="A16" s="48"/>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
@@ -1372,24 +1415,24 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="48" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="35"/>
+      <c r="A22" s="48"/>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="35"/>
+      <c r="A23" s="48"/>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="35"/>
+      <c r="A24" s="48"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="35"/>
+      <c r="A25" s="48"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="35"/>
+      <c r="A26" s="48"/>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="2"/>
@@ -1401,74 +1444,74 @@
       <c r="B29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="33"/>
-      <c r="N29" s="34"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="37"/>
     </row>
     <row r="30" spans="1:14">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="20">
+      <c r="B30" s="32">
         <v>44961</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="25"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="22"/>
     </row>
     <row r="31" spans="1:14">
-      <c r="A31" s="18"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="27"/>
-      <c r="N31" s="28"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
+      <c r="N31" s="25"/>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="19"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="30"/>
-      <c r="M32" s="30"/>
-      <c r="N32" s="31"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="27"/>
+      <c r="L32" s="27"/>
+      <c r="M32" s="27"/>
+      <c r="N32" s="28"/>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="3" t="s">
@@ -1477,74 +1520,74 @@
       <c r="B35" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="32" t="s">
+      <c r="C35" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="33"/>
-      <c r="K35" s="33"/>
-      <c r="L35" s="33"/>
-      <c r="M35" s="33"/>
-      <c r="N35" s="34"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="36"/>
+      <c r="J35" s="36"/>
+      <c r="K35" s="36"/>
+      <c r="L35" s="36"/>
+      <c r="M35" s="36"/>
+      <c r="N35" s="37"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="20">
+      <c r="B36" s="32">
         <v>44962</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="24"/>
-      <c r="L36" s="24"/>
-      <c r="M36" s="24"/>
-      <c r="N36" s="25"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="22"/>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="18"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="27"/>
-      <c r="N37" s="28"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="24"/>
+      <c r="N37" s="25"/>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="19"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="30"/>
-      <c r="M38" s="30"/>
-      <c r="N38" s="31"/>
+      <c r="A38" s="31"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="27"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
+      <c r="N38" s="28"/>
     </row>
     <row r="41" spans="1:14">
       <c r="A41" s="3" t="s">
@@ -1552,18 +1595,18 @@
       </c>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="15"/>
+      <c r="A43" s="13"/>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="15"/>
+      <c r="A44" s="13"/>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="15"/>
+      <c r="A45" s="13"/>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="3" t="s">
@@ -1571,15 +1614,15 @@
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="15"/>
+      <c r="A51" s="13"/>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="15"/>
+      <c r="A52" s="13"/>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="5" t="s">
@@ -1587,27 +1630,27 @@
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="36" t="s">
+      <c r="A56" s="38" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="36"/>
+      <c r="A57" s="38"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="36"/>
+      <c r="A58" s="38"/>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="36"/>
+      <c r="A59" s="38"/>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="36"/>
+      <c r="A60" s="38"/>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="36"/>
+      <c r="A61" s="38"/>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="36"/>
+      <c r="A62" s="38"/>
     </row>
     <row r="66" spans="1:14">
       <c r="A66" s="5" t="s">
@@ -1615,27 +1658,27 @@
       </c>
     </row>
     <row r="67" spans="1:14">
-      <c r="A67" s="36" t="s">
+      <c r="A67" s="38" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:14">
-      <c r="A68" s="36"/>
+      <c r="A68" s="38"/>
     </row>
     <row r="69" spans="1:14">
-      <c r="A69" s="36"/>
+      <c r="A69" s="38"/>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="36"/>
+      <c r="A70" s="38"/>
     </row>
     <row r="71" spans="1:14">
-      <c r="A71" s="36"/>
+      <c r="A71" s="38"/>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="36"/>
+      <c r="A72" s="38"/>
     </row>
     <row r="73" spans="1:14">
-      <c r="A73" s="36"/>
+      <c r="A73" s="38"/>
     </row>
     <row r="77" spans="1:14">
       <c r="A77" s="3" t="s">
@@ -1644,74 +1687,74 @@
       <c r="B77" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C77" s="32" t="s">
+      <c r="C77" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D77" s="33"/>
-      <c r="E77" s="33"/>
-      <c r="F77" s="33"/>
-      <c r="G77" s="33"/>
-      <c r="H77" s="33"/>
-      <c r="I77" s="33"/>
-      <c r="J77" s="33"/>
-      <c r="K77" s="33"/>
-      <c r="L77" s="33"/>
-      <c r="M77" s="33"/>
-      <c r="N77" s="34"/>
+      <c r="D77" s="36"/>
+      <c r="E77" s="36"/>
+      <c r="F77" s="36"/>
+      <c r="G77" s="36"/>
+      <c r="H77" s="36"/>
+      <c r="I77" s="36"/>
+      <c r="J77" s="36"/>
+      <c r="K77" s="36"/>
+      <c r="L77" s="36"/>
+      <c r="M77" s="36"/>
+      <c r="N77" s="37"/>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="17" t="s">
+      <c r="A78" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B78" s="20">
+      <c r="B78" s="32">
         <v>44967</v>
       </c>
-      <c r="C78" s="37" t="s">
+      <c r="C78" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="D78" s="38"/>
-      <c r="E78" s="38"/>
-      <c r="F78" s="38"/>
-      <c r="G78" s="38"/>
-      <c r="H78" s="38"/>
-      <c r="I78" s="38"/>
-      <c r="J78" s="38"/>
-      <c r="K78" s="38"/>
-      <c r="L78" s="38"/>
-      <c r="M78" s="38"/>
-      <c r="N78" s="39"/>
+      <c r="D78" s="40"/>
+      <c r="E78" s="40"/>
+      <c r="F78" s="40"/>
+      <c r="G78" s="40"/>
+      <c r="H78" s="40"/>
+      <c r="I78" s="40"/>
+      <c r="J78" s="40"/>
+      <c r="K78" s="40"/>
+      <c r="L78" s="40"/>
+      <c r="M78" s="40"/>
+      <c r="N78" s="41"/>
     </row>
     <row r="79" spans="1:14">
-      <c r="A79" s="18"/>
-      <c r="B79" s="21"/>
-      <c r="C79" s="40"/>
-      <c r="D79" s="41"/>
-      <c r="E79" s="41"/>
-      <c r="F79" s="41"/>
-      <c r="G79" s="41"/>
-      <c r="H79" s="41"/>
-      <c r="I79" s="41"/>
-      <c r="J79" s="41"/>
-      <c r="K79" s="41"/>
-      <c r="L79" s="41"/>
-      <c r="M79" s="41"/>
-      <c r="N79" s="42"/>
+      <c r="A79" s="30"/>
+      <c r="B79" s="33"/>
+      <c r="C79" s="42"/>
+      <c r="D79" s="43"/>
+      <c r="E79" s="43"/>
+      <c r="F79" s="43"/>
+      <c r="G79" s="43"/>
+      <c r="H79" s="43"/>
+      <c r="I79" s="43"/>
+      <c r="J79" s="43"/>
+      <c r="K79" s="43"/>
+      <c r="L79" s="43"/>
+      <c r="M79" s="43"/>
+      <c r="N79" s="44"/>
     </row>
     <row r="80" spans="1:14">
-      <c r="A80" s="19"/>
-      <c r="B80" s="22"/>
-      <c r="C80" s="43"/>
-      <c r="D80" s="44"/>
-      <c r="E80" s="44"/>
-      <c r="F80" s="44"/>
-      <c r="G80" s="44"/>
-      <c r="H80" s="44"/>
-      <c r="I80" s="44"/>
-      <c r="J80" s="44"/>
-      <c r="K80" s="44"/>
-      <c r="L80" s="44"/>
-      <c r="M80" s="44"/>
-      <c r="N80" s="45"/>
+      <c r="A80" s="31"/>
+      <c r="B80" s="34"/>
+      <c r="C80" s="45"/>
+      <c r="D80" s="46"/>
+      <c r="E80" s="46"/>
+      <c r="F80" s="46"/>
+      <c r="G80" s="46"/>
+      <c r="H80" s="46"/>
+      <c r="I80" s="46"/>
+      <c r="J80" s="46"/>
+      <c r="K80" s="46"/>
+      <c r="L80" s="46"/>
+      <c r="M80" s="46"/>
+      <c r="N80" s="47"/>
     </row>
     <row r="83" spans="1:14">
       <c r="A83" s="3" t="s">
@@ -1720,74 +1763,74 @@
       <c r="B83" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C83" s="32" t="s">
+      <c r="C83" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D83" s="33"/>
-      <c r="E83" s="33"/>
-      <c r="F83" s="33"/>
-      <c r="G83" s="33"/>
-      <c r="H83" s="33"/>
-      <c r="I83" s="33"/>
-      <c r="J83" s="33"/>
-      <c r="K83" s="33"/>
-      <c r="L83" s="33"/>
-      <c r="M83" s="33"/>
-      <c r="N83" s="34"/>
+      <c r="D83" s="36"/>
+      <c r="E83" s="36"/>
+      <c r="F83" s="36"/>
+      <c r="G83" s="36"/>
+      <c r="H83" s="36"/>
+      <c r="I83" s="36"/>
+      <c r="J83" s="36"/>
+      <c r="K83" s="36"/>
+      <c r="L83" s="36"/>
+      <c r="M83" s="36"/>
+      <c r="N83" s="37"/>
     </row>
     <row r="84" spans="1:14">
-      <c r="A84" s="17" t="s">
+      <c r="A84" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B84" s="20">
+      <c r="B84" s="32">
         <v>44968</v>
       </c>
-      <c r="C84" s="23" t="s">
+      <c r="C84" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D84" s="24"/>
-      <c r="E84" s="24"/>
-      <c r="F84" s="24"/>
-      <c r="G84" s="24"/>
-      <c r="H84" s="24"/>
-      <c r="I84" s="24"/>
-      <c r="J84" s="24"/>
-      <c r="K84" s="24"/>
-      <c r="L84" s="24"/>
-      <c r="M84" s="24"/>
-      <c r="N84" s="25"/>
+      <c r="D84" s="21"/>
+      <c r="E84" s="21"/>
+      <c r="F84" s="21"/>
+      <c r="G84" s="21"/>
+      <c r="H84" s="21"/>
+      <c r="I84" s="21"/>
+      <c r="J84" s="21"/>
+      <c r="K84" s="21"/>
+      <c r="L84" s="21"/>
+      <c r="M84" s="21"/>
+      <c r="N84" s="22"/>
     </row>
     <row r="85" spans="1:14">
-      <c r="A85" s="18"/>
-      <c r="B85" s="21"/>
-      <c r="C85" s="26"/>
-      <c r="D85" s="27"/>
-      <c r="E85" s="27"/>
-      <c r="F85" s="27"/>
-      <c r="G85" s="27"/>
-      <c r="H85" s="27"/>
-      <c r="I85" s="27"/>
-      <c r="J85" s="27"/>
-      <c r="K85" s="27"/>
-      <c r="L85" s="27"/>
-      <c r="M85" s="27"/>
-      <c r="N85" s="28"/>
+      <c r="A85" s="30"/>
+      <c r="B85" s="33"/>
+      <c r="C85" s="23"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="24"/>
+      <c r="H85" s="24"/>
+      <c r="I85" s="24"/>
+      <c r="J85" s="24"/>
+      <c r="K85" s="24"/>
+      <c r="L85" s="24"/>
+      <c r="M85" s="24"/>
+      <c r="N85" s="25"/>
     </row>
     <row r="86" spans="1:14">
-      <c r="A86" s="19"/>
-      <c r="B86" s="22"/>
-      <c r="C86" s="29"/>
-      <c r="D86" s="30"/>
-      <c r="E86" s="30"/>
-      <c r="F86" s="30"/>
-      <c r="G86" s="30"/>
-      <c r="H86" s="30"/>
-      <c r="I86" s="30"/>
-      <c r="J86" s="30"/>
-      <c r="K86" s="30"/>
-      <c r="L86" s="30"/>
-      <c r="M86" s="30"/>
-      <c r="N86" s="31"/>
+      <c r="A86" s="31"/>
+      <c r="B86" s="34"/>
+      <c r="C86" s="26"/>
+      <c r="D86" s="27"/>
+      <c r="E86" s="27"/>
+      <c r="F86" s="27"/>
+      <c r="G86" s="27"/>
+      <c r="H86" s="27"/>
+      <c r="I86" s="27"/>
+      <c r="J86" s="27"/>
+      <c r="K86" s="27"/>
+      <c r="L86" s="27"/>
+      <c r="M86" s="27"/>
+      <c r="N86" s="28"/>
     </row>
     <row r="89" spans="1:14">
       <c r="A89" s="3" t="s">
@@ -1796,74 +1839,74 @@
       <c r="B89" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C89" s="32" t="s">
+      <c r="C89" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D89" s="33"/>
-      <c r="E89" s="33"/>
-      <c r="F89" s="33"/>
-      <c r="G89" s="33"/>
-      <c r="H89" s="33"/>
-      <c r="I89" s="33"/>
-      <c r="J89" s="33"/>
-      <c r="K89" s="33"/>
-      <c r="L89" s="33"/>
-      <c r="M89" s="33"/>
-      <c r="N89" s="34"/>
+      <c r="D89" s="36"/>
+      <c r="E89" s="36"/>
+      <c r="F89" s="36"/>
+      <c r="G89" s="36"/>
+      <c r="H89" s="36"/>
+      <c r="I89" s="36"/>
+      <c r="J89" s="36"/>
+      <c r="K89" s="36"/>
+      <c r="L89" s="36"/>
+      <c r="M89" s="36"/>
+      <c r="N89" s="37"/>
     </row>
     <row r="90" spans="1:14">
-      <c r="A90" s="17" t="s">
+      <c r="A90" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B90" s="20">
+      <c r="B90" s="32">
         <v>44969</v>
       </c>
-      <c r="C90" s="23" t="s">
+      <c r="C90" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D90" s="24"/>
-      <c r="E90" s="24"/>
-      <c r="F90" s="24"/>
-      <c r="G90" s="24"/>
-      <c r="H90" s="24"/>
-      <c r="I90" s="24"/>
-      <c r="J90" s="24"/>
-      <c r="K90" s="24"/>
-      <c r="L90" s="24"/>
-      <c r="M90" s="24"/>
-      <c r="N90" s="25"/>
+      <c r="D90" s="21"/>
+      <c r="E90" s="21"/>
+      <c r="F90" s="21"/>
+      <c r="G90" s="21"/>
+      <c r="H90" s="21"/>
+      <c r="I90" s="21"/>
+      <c r="J90" s="21"/>
+      <c r="K90" s="21"/>
+      <c r="L90" s="21"/>
+      <c r="M90" s="21"/>
+      <c r="N90" s="22"/>
     </row>
     <row r="91" spans="1:14">
-      <c r="A91" s="18"/>
-      <c r="B91" s="21"/>
-      <c r="C91" s="26"/>
-      <c r="D91" s="27"/>
-      <c r="E91" s="27"/>
-      <c r="F91" s="27"/>
-      <c r="G91" s="27"/>
-      <c r="H91" s="27"/>
-      <c r="I91" s="27"/>
-      <c r="J91" s="27"/>
-      <c r="K91" s="27"/>
-      <c r="L91" s="27"/>
-      <c r="M91" s="27"/>
-      <c r="N91" s="28"/>
+      <c r="A91" s="30"/>
+      <c r="B91" s="33"/>
+      <c r="C91" s="23"/>
+      <c r="D91" s="24"/>
+      <c r="E91" s="24"/>
+      <c r="F91" s="24"/>
+      <c r="G91" s="24"/>
+      <c r="H91" s="24"/>
+      <c r="I91" s="24"/>
+      <c r="J91" s="24"/>
+      <c r="K91" s="24"/>
+      <c r="L91" s="24"/>
+      <c r="M91" s="24"/>
+      <c r="N91" s="25"/>
     </row>
     <row r="92" spans="1:14">
-      <c r="A92" s="19"/>
-      <c r="B92" s="22"/>
-      <c r="C92" s="29"/>
-      <c r="D92" s="30"/>
-      <c r="E92" s="30"/>
-      <c r="F92" s="30"/>
-      <c r="G92" s="30"/>
-      <c r="H92" s="30"/>
-      <c r="I92" s="30"/>
-      <c r="J92" s="30"/>
-      <c r="K92" s="30"/>
-      <c r="L92" s="30"/>
-      <c r="M92" s="30"/>
-      <c r="N92" s="31"/>
+      <c r="A92" s="31"/>
+      <c r="B92" s="34"/>
+      <c r="C92" s="26"/>
+      <c r="D92" s="27"/>
+      <c r="E92" s="27"/>
+      <c r="F92" s="27"/>
+      <c r="G92" s="27"/>
+      <c r="H92" s="27"/>
+      <c r="I92" s="27"/>
+      <c r="J92" s="27"/>
+      <c r="K92" s="27"/>
+      <c r="L92" s="27"/>
+      <c r="M92" s="27"/>
+      <c r="N92" s="28"/>
     </row>
     <row r="144" spans="1:14">
       <c r="A144" s="3" t="s">
@@ -1872,74 +1915,74 @@
       <c r="B144" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C144" s="6" t="s">
+      <c r="C144" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D144" s="7"/>
-      <c r="E144" s="7"/>
-      <c r="F144" s="7"/>
-      <c r="G144" s="7"/>
-      <c r="H144" s="7"/>
-      <c r="I144" s="7"/>
-      <c r="J144" s="7"/>
-      <c r="K144" s="7"/>
-      <c r="L144" s="7"/>
-      <c r="M144" s="7"/>
-      <c r="N144" s="8"/>
+      <c r="D144" s="50"/>
+      <c r="E144" s="50"/>
+      <c r="F144" s="50"/>
+      <c r="G144" s="50"/>
+      <c r="H144" s="50"/>
+      <c r="I144" s="50"/>
+      <c r="J144" s="50"/>
+      <c r="K144" s="50"/>
+      <c r="L144" s="50"/>
+      <c r="M144" s="50"/>
+      <c r="N144" s="51"/>
     </row>
     <row r="145" spans="1:14">
-      <c r="A145" s="17" t="s">
+      <c r="A145" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B145" s="20">
+      <c r="B145" s="32">
         <v>44975</v>
       </c>
-      <c r="C145" s="23" t="s">
+      <c r="C145" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D145" s="24"/>
-      <c r="E145" s="24"/>
-      <c r="F145" s="24"/>
-      <c r="G145" s="24"/>
-      <c r="H145" s="24"/>
-      <c r="I145" s="24"/>
-      <c r="J145" s="24"/>
-      <c r="K145" s="24"/>
-      <c r="L145" s="24"/>
-      <c r="M145" s="24"/>
-      <c r="N145" s="25"/>
+      <c r="D145" s="21"/>
+      <c r="E145" s="21"/>
+      <c r="F145" s="21"/>
+      <c r="G145" s="21"/>
+      <c r="H145" s="21"/>
+      <c r="I145" s="21"/>
+      <c r="J145" s="21"/>
+      <c r="K145" s="21"/>
+      <c r="L145" s="21"/>
+      <c r="M145" s="21"/>
+      <c r="N145" s="22"/>
     </row>
     <row r="146" spans="1:14">
-      <c r="A146" s="18"/>
-      <c r="B146" s="21"/>
-      <c r="C146" s="26"/>
-      <c r="D146" s="27"/>
-      <c r="E146" s="27"/>
-      <c r="F146" s="27"/>
-      <c r="G146" s="27"/>
-      <c r="H146" s="27"/>
-      <c r="I146" s="27"/>
-      <c r="J146" s="27"/>
-      <c r="K146" s="27"/>
-      <c r="L146" s="27"/>
-      <c r="M146" s="27"/>
-      <c r="N146" s="28"/>
+      <c r="A146" s="30"/>
+      <c r="B146" s="33"/>
+      <c r="C146" s="23"/>
+      <c r="D146" s="24"/>
+      <c r="E146" s="24"/>
+      <c r="F146" s="24"/>
+      <c r="G146" s="24"/>
+      <c r="H146" s="24"/>
+      <c r="I146" s="24"/>
+      <c r="J146" s="24"/>
+      <c r="K146" s="24"/>
+      <c r="L146" s="24"/>
+      <c r="M146" s="24"/>
+      <c r="N146" s="25"/>
     </row>
     <row r="147" spans="1:14">
-      <c r="A147" s="19"/>
-      <c r="B147" s="22"/>
-      <c r="C147" s="29"/>
-      <c r="D147" s="30"/>
-      <c r="E147" s="30"/>
-      <c r="F147" s="30"/>
-      <c r="G147" s="30"/>
-      <c r="H147" s="30"/>
-      <c r="I147" s="30"/>
-      <c r="J147" s="30"/>
-      <c r="K147" s="30"/>
-      <c r="L147" s="30"/>
-      <c r="M147" s="30"/>
-      <c r="N147" s="31"/>
+      <c r="A147" s="31"/>
+      <c r="B147" s="34"/>
+      <c r="C147" s="26"/>
+      <c r="D147" s="27"/>
+      <c r="E147" s="27"/>
+      <c r="F147" s="27"/>
+      <c r="G147" s="27"/>
+      <c r="H147" s="27"/>
+      <c r="I147" s="27"/>
+      <c r="J147" s="27"/>
+      <c r="K147" s="27"/>
+      <c r="L147" s="27"/>
+      <c r="M147" s="27"/>
+      <c r="N147" s="28"/>
     </row>
     <row r="150" spans="1:14">
       <c r="A150" s="3" t="s">
@@ -1948,74 +1991,74 @@
       <c r="B150" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C150" s="6" t="s">
+      <c r="C150" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D150" s="7"/>
-      <c r="E150" s="7"/>
-      <c r="F150" s="7"/>
-      <c r="G150" s="7"/>
-      <c r="H150" s="7"/>
-      <c r="I150" s="7"/>
-      <c r="J150" s="7"/>
-      <c r="K150" s="7"/>
-      <c r="L150" s="7"/>
-      <c r="M150" s="7"/>
-      <c r="N150" s="8"/>
+      <c r="D150" s="36"/>
+      <c r="E150" s="36"/>
+      <c r="F150" s="36"/>
+      <c r="G150" s="36"/>
+      <c r="H150" s="36"/>
+      <c r="I150" s="36"/>
+      <c r="J150" s="36"/>
+      <c r="K150" s="36"/>
+      <c r="L150" s="36"/>
+      <c r="M150" s="36"/>
+      <c r="N150" s="37"/>
     </row>
     <row r="151" spans="1:14">
-      <c r="A151" s="17" t="s">
+      <c r="A151" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B151" s="20">
+      <c r="B151" s="32">
         <v>44976</v>
       </c>
-      <c r="C151" s="23" t="s">
+      <c r="C151" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D151" s="24"/>
-      <c r="E151" s="24"/>
-      <c r="F151" s="24"/>
-      <c r="G151" s="24"/>
-      <c r="H151" s="24"/>
-      <c r="I151" s="24"/>
-      <c r="J151" s="24"/>
-      <c r="K151" s="24"/>
-      <c r="L151" s="24"/>
-      <c r="M151" s="24"/>
-      <c r="N151" s="25"/>
+      <c r="D151" s="21"/>
+      <c r="E151" s="21"/>
+      <c r="F151" s="21"/>
+      <c r="G151" s="21"/>
+      <c r="H151" s="21"/>
+      <c r="I151" s="21"/>
+      <c r="J151" s="21"/>
+      <c r="K151" s="21"/>
+      <c r="L151" s="21"/>
+      <c r="M151" s="21"/>
+      <c r="N151" s="22"/>
     </row>
     <row r="152" spans="1:14">
-      <c r="A152" s="18"/>
-      <c r="B152" s="21"/>
-      <c r="C152" s="26"/>
-      <c r="D152" s="27"/>
-      <c r="E152" s="27"/>
-      <c r="F152" s="27"/>
-      <c r="G152" s="27"/>
-      <c r="H152" s="27"/>
-      <c r="I152" s="27"/>
-      <c r="J152" s="27"/>
-      <c r="K152" s="27"/>
-      <c r="L152" s="27"/>
-      <c r="M152" s="27"/>
-      <c r="N152" s="28"/>
+      <c r="A152" s="30"/>
+      <c r="B152" s="33"/>
+      <c r="C152" s="23"/>
+      <c r="D152" s="24"/>
+      <c r="E152" s="24"/>
+      <c r="F152" s="24"/>
+      <c r="G152" s="24"/>
+      <c r="H152" s="24"/>
+      <c r="I152" s="24"/>
+      <c r="J152" s="24"/>
+      <c r="K152" s="24"/>
+      <c r="L152" s="24"/>
+      <c r="M152" s="24"/>
+      <c r="N152" s="25"/>
     </row>
     <row r="153" spans="1:14">
-      <c r="A153" s="19"/>
-      <c r="B153" s="22"/>
-      <c r="C153" s="29"/>
-      <c r="D153" s="30"/>
-      <c r="E153" s="30"/>
-      <c r="F153" s="30"/>
-      <c r="G153" s="30"/>
-      <c r="H153" s="30"/>
-      <c r="I153" s="30"/>
-      <c r="J153" s="30"/>
-      <c r="K153" s="30"/>
-      <c r="L153" s="30"/>
-      <c r="M153" s="30"/>
-      <c r="N153" s="31"/>
+      <c r="A153" s="31"/>
+      <c r="B153" s="34"/>
+      <c r="C153" s="26"/>
+      <c r="D153" s="27"/>
+      <c r="E153" s="27"/>
+      <c r="F153" s="27"/>
+      <c r="G153" s="27"/>
+      <c r="H153" s="27"/>
+      <c r="I153" s="27"/>
+      <c r="J153" s="27"/>
+      <c r="K153" s="27"/>
+      <c r="L153" s="27"/>
+      <c r="M153" s="27"/>
+      <c r="N153" s="28"/>
     </row>
     <row r="156" spans="1:14">
       <c r="A156" s="3" t="s">
@@ -2033,117 +2076,117 @@
       <c r="E156" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F156" s="46" t="s">
+      <c r="F156" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G156" s="47"/>
-      <c r="H156" s="47"/>
-      <c r="I156" s="47"/>
-      <c r="J156" s="47"/>
-      <c r="K156" s="47"/>
-      <c r="L156" s="47"/>
-      <c r="M156" s="47"/>
-      <c r="N156" s="47"/>
+      <c r="G156" s="12"/>
+      <c r="H156" s="12"/>
+      <c r="I156" s="12"/>
+      <c r="J156" s="12"/>
+      <c r="K156" s="12"/>
+      <c r="L156" s="12"/>
+      <c r="M156" s="12"/>
+      <c r="N156" s="12"/>
     </row>
     <row r="157" spans="1:14">
-      <c r="A157" s="15" t="s">
+      <c r="A157" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B157" s="16">
+      <c r="B157" s="14">
         <v>44977</v>
       </c>
-      <c r="C157" s="9" t="s">
+      <c r="C157" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D157" s="9">
+      <c r="D157" s="6">
         <v>0.39583333333333331</v>
       </c>
-      <c r="E157" s="9">
+      <c r="E157" s="6">
         <v>0.40277777777777773</v>
       </c>
-      <c r="F157" s="13" t="s">
+      <c r="F157" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G157" s="13"/>
-      <c r="H157" s="13"/>
-      <c r="I157" s="13"/>
-      <c r="J157" s="13"/>
-      <c r="K157" s="13"/>
-      <c r="L157" s="13"/>
-      <c r="M157" s="13"/>
-      <c r="N157" s="13"/>
+      <c r="G157" s="15"/>
+      <c r="H157" s="15"/>
+      <c r="I157" s="15"/>
+      <c r="J157" s="15"/>
+      <c r="K157" s="15"/>
+      <c r="L157" s="15"/>
+      <c r="M157" s="15"/>
+      <c r="N157" s="15"/>
     </row>
     <row r="158" spans="1:14">
-      <c r="A158" s="15"/>
-      <c r="B158" s="16"/>
-      <c r="C158" s="9" t="s">
+      <c r="A158" s="13"/>
+      <c r="B158" s="14"/>
+      <c r="C158" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D158" s="9">
+      <c r="D158" s="6">
         <v>0.40277777777777773</v>
       </c>
-      <c r="E158" s="9">
+      <c r="E158" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F158" s="13" t="s">
+      <c r="F158" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G158" s="13"/>
-      <c r="H158" s="13"/>
-      <c r="I158" s="13"/>
-      <c r="J158" s="13"/>
-      <c r="K158" s="13"/>
-      <c r="L158" s="13"/>
-      <c r="M158" s="13"/>
-      <c r="N158" s="13"/>
+      <c r="G158" s="15"/>
+      <c r="H158" s="15"/>
+      <c r="I158" s="15"/>
+      <c r="J158" s="15"/>
+      <c r="K158" s="15"/>
+      <c r="L158" s="15"/>
+      <c r="M158" s="15"/>
+      <c r="N158" s="15"/>
     </row>
     <row r="159" spans="1:14">
-      <c r="A159" s="15"/>
-      <c r="B159" s="16"/>
-      <c r="C159" s="10" t="s">
+      <c r="A159" s="13"/>
+      <c r="B159" s="14"/>
+      <c r="C159" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D159" s="9">
+      <c r="D159" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E159" s="9">
+      <c r="E159" s="6">
         <v>0.22916666666666666</v>
       </c>
-      <c r="F159" s="48" t="s">
+      <c r="F159" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G159" s="49"/>
-      <c r="H159" s="49"/>
-      <c r="I159" s="49"/>
-      <c r="J159" s="49"/>
-      <c r="K159" s="49"/>
-      <c r="L159" s="49"/>
-      <c r="M159" s="49"/>
-      <c r="N159" s="50"/>
+      <c r="G159" s="17"/>
+      <c r="H159" s="17"/>
+      <c r="I159" s="17"/>
+      <c r="J159" s="17"/>
+      <c r="K159" s="17"/>
+      <c r="L159" s="17"/>
+      <c r="M159" s="17"/>
+      <c r="N159" s="18"/>
     </row>
     <row r="160" spans="1:14">
-      <c r="A160" s="15"/>
-      <c r="B160" s="16"/>
-      <c r="C160" s="10" t="s">
+      <c r="A160" s="13"/>
+      <c r="B160" s="14"/>
+      <c r="C160" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D160" s="9">
+      <c r="D160" s="6">
         <v>0.22916666666666666</v>
       </c>
-      <c r="E160" s="9">
+      <c r="E160" s="6">
         <v>0.27083333333333331</v>
       </c>
-      <c r="F160" s="13" t="s">
+      <c r="F160" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G160" s="13"/>
-      <c r="H160" s="13"/>
-      <c r="I160" s="13"/>
-      <c r="J160" s="13"/>
-      <c r="K160" s="13"/>
-      <c r="L160" s="13"/>
-      <c r="M160" s="13"/>
-      <c r="N160" s="13"/>
+      <c r="G160" s="15"/>
+      <c r="H160" s="15"/>
+      <c r="I160" s="15"/>
+      <c r="J160" s="15"/>
+      <c r="K160" s="15"/>
+      <c r="L160" s="15"/>
+      <c r="M160" s="15"/>
+      <c r="N160" s="15"/>
     </row>
     <row r="163" spans="1:14">
       <c r="A163" s="3" t="s">
@@ -2161,93 +2204,93 @@
       <c r="E163" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F163" s="14" t="s">
+      <c r="F163" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G163" s="14"/>
-      <c r="H163" s="14"/>
-      <c r="I163" s="14"/>
-      <c r="J163" s="14"/>
-      <c r="K163" s="14"/>
-      <c r="L163" s="14"/>
-      <c r="M163" s="14"/>
-      <c r="N163" s="14"/>
+      <c r="G163" s="19"/>
+      <c r="H163" s="19"/>
+      <c r="I163" s="19"/>
+      <c r="J163" s="19"/>
+      <c r="K163" s="19"/>
+      <c r="L163" s="19"/>
+      <c r="M163" s="19"/>
+      <c r="N163" s="19"/>
     </row>
     <row r="164" spans="1:14">
-      <c r="A164" s="15" t="s">
+      <c r="A164" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B164" s="16">
+      <c r="B164" s="14">
         <v>44978</v>
       </c>
-      <c r="C164" s="9" t="s">
+      <c r="C164" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D164" s="9">
+      <c r="D164" s="6">
         <v>0.39583333333333331</v>
       </c>
-      <c r="E164" s="9">
+      <c r="E164" s="6">
         <v>0.40277777777777773</v>
       </c>
-      <c r="F164" s="13" t="s">
+      <c r="F164" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G164" s="13"/>
-      <c r="H164" s="13"/>
-      <c r="I164" s="13"/>
-      <c r="J164" s="13"/>
-      <c r="K164" s="13"/>
-      <c r="L164" s="13"/>
-      <c r="M164" s="13"/>
-      <c r="N164" s="13"/>
+      <c r="G164" s="15"/>
+      <c r="H164" s="15"/>
+      <c r="I164" s="15"/>
+      <c r="J164" s="15"/>
+      <c r="K164" s="15"/>
+      <c r="L164" s="15"/>
+      <c r="M164" s="15"/>
+      <c r="N164" s="15"/>
     </row>
     <row r="165" spans="1:14">
-      <c r="A165" s="15"/>
-      <c r="B165" s="16"/>
-      <c r="C165" s="10" t="s">
+      <c r="A165" s="13"/>
+      <c r="B165" s="14"/>
+      <c r="C165" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D165" s="9">
+      <c r="D165" s="6">
         <v>0.40277777777777773</v>
       </c>
-      <c r="E165" s="9">
+      <c r="E165" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F165" s="13" t="s">
+      <c r="F165" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G165" s="13"/>
-      <c r="H165" s="13"/>
-      <c r="I165" s="13"/>
-      <c r="J165" s="13"/>
-      <c r="K165" s="13"/>
-      <c r="L165" s="13"/>
-      <c r="M165" s="13"/>
-      <c r="N165" s="13"/>
+      <c r="G165" s="15"/>
+      <c r="H165" s="15"/>
+      <c r="I165" s="15"/>
+      <c r="J165" s="15"/>
+      <c r="K165" s="15"/>
+      <c r="L165" s="15"/>
+      <c r="M165" s="15"/>
+      <c r="N165" s="15"/>
     </row>
     <row r="166" spans="1:14">
-      <c r="A166" s="15"/>
-      <c r="B166" s="16"/>
-      <c r="C166" s="10" t="s">
+      <c r="A166" s="13"/>
+      <c r="B166" s="14"/>
+      <c r="C166" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D166" s="9">
+      <c r="D166" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E166" s="9">
+      <c r="E166" s="6">
         <v>0.27083333333333331</v>
       </c>
-      <c r="F166" s="13" t="s">
+      <c r="F166" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G166" s="13"/>
-      <c r="H166" s="13"/>
-      <c r="I166" s="13"/>
-      <c r="J166" s="13"/>
-      <c r="K166" s="13"/>
-      <c r="L166" s="13"/>
-      <c r="M166" s="13"/>
-      <c r="N166" s="13"/>
+      <c r="G166" s="15"/>
+      <c r="H166" s="15"/>
+      <c r="I166" s="15"/>
+      <c r="J166" s="15"/>
+      <c r="K166" s="15"/>
+      <c r="L166" s="15"/>
+      <c r="M166" s="15"/>
+      <c r="N166" s="15"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="4" t="s">
@@ -2265,318 +2308,663 @@
       <c r="E169" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F169" s="14" t="s">
+      <c r="F169" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G169" s="14"/>
-      <c r="H169" s="14"/>
-      <c r="I169" s="14"/>
-      <c r="J169" s="14"/>
-      <c r="K169" s="14"/>
-      <c r="L169" s="14"/>
-      <c r="M169" s="14"/>
-      <c r="N169" s="14"/>
+      <c r="G169" s="19"/>
+      <c r="H169" s="19"/>
+      <c r="I169" s="19"/>
+      <c r="J169" s="19"/>
+      <c r="K169" s="19"/>
+      <c r="L169" s="19"/>
+      <c r="M169" s="19"/>
+      <c r="N169" s="19"/>
     </row>
     <row r="170" spans="1:14">
-      <c r="A170" s="15" t="s">
+      <c r="A170" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B170" s="16">
+      <c r="B170" s="14">
         <v>44979</v>
       </c>
-      <c r="C170" s="9" t="s">
+      <c r="C170" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D170" s="9">
+      <c r="D170" s="6">
         <v>0.39583333333333331</v>
       </c>
-      <c r="E170" s="9">
+      <c r="E170" s="6">
         <v>0.40277777777777773</v>
       </c>
-      <c r="F170" s="13" t="s">
+      <c r="F170" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G170" s="13"/>
-      <c r="H170" s="13"/>
-      <c r="I170" s="13"/>
-      <c r="J170" s="13"/>
-      <c r="K170" s="13"/>
-      <c r="L170" s="13"/>
-      <c r="M170" s="13"/>
-      <c r="N170" s="13"/>
+      <c r="G170" s="15"/>
+      <c r="H170" s="15"/>
+      <c r="I170" s="15"/>
+      <c r="J170" s="15"/>
+      <c r="K170" s="15"/>
+      <c r="L170" s="15"/>
+      <c r="M170" s="15"/>
+      <c r="N170" s="15"/>
     </row>
     <row r="171" spans="1:14">
-      <c r="A171" s="15"/>
-      <c r="B171" s="16"/>
-      <c r="C171" s="10" t="s">
+      <c r="A171" s="13"/>
+      <c r="B171" s="14"/>
+      <c r="C171" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D171" s="9">
+      <c r="D171" s="6">
         <v>0.40277777777777773</v>
       </c>
-      <c r="E171" s="9">
+      <c r="E171" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F171" s="13" t="s">
+      <c r="F171" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G171" s="13"/>
-      <c r="H171" s="13"/>
-      <c r="I171" s="13"/>
-      <c r="J171" s="13"/>
-      <c r="K171" s="13"/>
-      <c r="L171" s="13"/>
-      <c r="M171" s="13"/>
-      <c r="N171" s="13"/>
+      <c r="G171" s="15"/>
+      <c r="H171" s="15"/>
+      <c r="I171" s="15"/>
+      <c r="J171" s="15"/>
+      <c r="K171" s="15"/>
+      <c r="L171" s="15"/>
+      <c r="M171" s="15"/>
+      <c r="N171" s="15"/>
     </row>
     <row r="172" spans="1:14">
-      <c r="A172" s="15"/>
-      <c r="B172" s="16"/>
-      <c r="C172" s="10" t="s">
+      <c r="A172" s="13"/>
+      <c r="B172" s="14"/>
+      <c r="C172" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D172" s="9">
+      <c r="D172" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E172" s="9">
+      <c r="E172" s="6">
         <v>0.27083333333333331</v>
       </c>
-      <c r="F172" s="13" t="s">
+      <c r="F172" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G172" s="13"/>
-      <c r="H172" s="13"/>
-      <c r="I172" s="13"/>
-      <c r="J172" s="13"/>
-      <c r="K172" s="13"/>
-      <c r="L172" s="13"/>
-      <c r="M172" s="13"/>
-      <c r="N172" s="13"/>
+      <c r="G172" s="15"/>
+      <c r="H172" s="15"/>
+      <c r="I172" s="15"/>
+      <c r="J172" s="15"/>
+      <c r="K172" s="15"/>
+      <c r="L172" s="15"/>
+      <c r="M172" s="15"/>
+      <c r="N172" s="15"/>
     </row>
     <row r="175" spans="1:14">
-      <c r="A175" s="11" t="s">
+      <c r="A175" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B175" s="11" t="s">
+      <c r="B175" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C175" s="11" t="s">
+      <c r="C175" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D175" s="11" t="s">
+      <c r="D175" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E175" s="11" t="s">
+      <c r="E175" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F175" s="14" t="s">
+      <c r="F175" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G175" s="14"/>
-      <c r="H175" s="14"/>
-      <c r="I175" s="14"/>
-      <c r="J175" s="14"/>
-      <c r="K175" s="14"/>
-      <c r="L175" s="14"/>
-      <c r="M175" s="14"/>
-      <c r="N175" s="14"/>
+      <c r="G175" s="19"/>
+      <c r="H175" s="19"/>
+      <c r="I175" s="19"/>
+      <c r="J175" s="19"/>
+      <c r="K175" s="19"/>
+      <c r="L175" s="19"/>
+      <c r="M175" s="19"/>
+      <c r="N175" s="19"/>
     </row>
     <row r="176" spans="1:14">
-      <c r="A176" s="15" t="s">
+      <c r="A176" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B176" s="16">
+      <c r="B176" s="14">
         <v>44980</v>
       </c>
-      <c r="C176" s="12" t="s">
+      <c r="C176" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D176" s="9">
+      <c r="D176" s="6">
         <v>0.39583333333333331</v>
       </c>
-      <c r="E176" s="9">
+      <c r="E176" s="6">
         <v>0.40277777777777773</v>
       </c>
-      <c r="F176" s="13" t="s">
+      <c r="F176" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G176" s="13"/>
-      <c r="H176" s="13"/>
-      <c r="I176" s="13"/>
-      <c r="J176" s="13"/>
-      <c r="K176" s="13"/>
-      <c r="L176" s="13"/>
-      <c r="M176" s="13"/>
-      <c r="N176" s="13"/>
+      <c r="G176" s="15"/>
+      <c r="H176" s="15"/>
+      <c r="I176" s="15"/>
+      <c r="J176" s="15"/>
+      <c r="K176" s="15"/>
+      <c r="L176" s="15"/>
+      <c r="M176" s="15"/>
+      <c r="N176" s="15"/>
     </row>
     <row r="177" spans="1:14">
-      <c r="A177" s="15"/>
-      <c r="B177" s="16"/>
-      <c r="C177" s="12" t="s">
+      <c r="A177" s="13"/>
+      <c r="B177" s="14"/>
+      <c r="C177" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D177" s="9">
+      <c r="D177" s="6">
         <v>0.40277777777777773</v>
       </c>
-      <c r="E177" s="9">
+      <c r="E177" s="6">
         <v>0.48125000000000001</v>
       </c>
-      <c r="F177" s="13" t="s">
+      <c r="F177" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G177" s="13"/>
-      <c r="H177" s="13"/>
-      <c r="I177" s="13"/>
-      <c r="J177" s="13"/>
-      <c r="K177" s="13"/>
-      <c r="L177" s="13"/>
-      <c r="M177" s="13"/>
-      <c r="N177" s="13"/>
+      <c r="G177" s="15"/>
+      <c r="H177" s="15"/>
+      <c r="I177" s="15"/>
+      <c r="J177" s="15"/>
+      <c r="K177" s="15"/>
+      <c r="L177" s="15"/>
+      <c r="M177" s="15"/>
+      <c r="N177" s="15"/>
     </row>
     <row r="178" spans="1:14">
-      <c r="A178" s="15"/>
-      <c r="B178" s="16"/>
-      <c r="C178" s="12" t="s">
+      <c r="A178" s="13"/>
+      <c r="B178" s="14"/>
+      <c r="C178" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D178" s="9">
+      <c r="D178" s="6">
         <v>0.48125000000000001</v>
       </c>
-      <c r="E178" s="9">
+      <c r="E178" s="6">
         <v>0.5</v>
       </c>
-      <c r="F178" s="13" t="s">
+      <c r="F178" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="G178" s="13"/>
-      <c r="H178" s="13"/>
-      <c r="I178" s="13"/>
-      <c r="J178" s="13"/>
-      <c r="K178" s="13"/>
-      <c r="L178" s="13"/>
-      <c r="M178" s="13"/>
-      <c r="N178" s="13"/>
+      <c r="G178" s="15"/>
+      <c r="H178" s="15"/>
+      <c r="I178" s="15"/>
+      <c r="J178" s="15"/>
+      <c r="K178" s="15"/>
+      <c r="L178" s="15"/>
+      <c r="M178" s="15"/>
+      <c r="N178" s="15"/>
     </row>
     <row r="179" spans="1:14">
-      <c r="A179" s="15"/>
-      <c r="B179" s="16"/>
-      <c r="C179" s="12" t="s">
+      <c r="A179" s="13"/>
+      <c r="B179" s="14"/>
+      <c r="C179" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D179" s="9">
+      <c r="D179" s="6">
         <v>0.5</v>
       </c>
-      <c r="E179" s="9">
+      <c r="E179" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F179" s="13" t="s">
+      <c r="F179" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G179" s="13"/>
-      <c r="H179" s="13"/>
-      <c r="I179" s="13"/>
-      <c r="J179" s="13"/>
-      <c r="K179" s="13"/>
-      <c r="L179" s="13"/>
-      <c r="M179" s="13"/>
-      <c r="N179" s="13"/>
+      <c r="G179" s="15"/>
+      <c r="H179" s="15"/>
+      <c r="I179" s="15"/>
+      <c r="J179" s="15"/>
+      <c r="K179" s="15"/>
+      <c r="L179" s="15"/>
+      <c r="M179" s="15"/>
+      <c r="N179" s="15"/>
     </row>
     <row r="180" spans="1:14">
-      <c r="A180" s="15"/>
-      <c r="B180" s="16"/>
-      <c r="C180" s="12" t="s">
+      <c r="A180" s="13"/>
+      <c r="B180" s="14"/>
+      <c r="C180" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D180" s="9">
+      <c r="D180" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E180" s="9">
+      <c r="E180" s="6">
         <v>0.125</v>
       </c>
-      <c r="F180" s="13" t="s">
+      <c r="F180" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G180" s="13"/>
-      <c r="H180" s="13"/>
-      <c r="I180" s="13"/>
-      <c r="J180" s="13"/>
-      <c r="K180" s="13"/>
-      <c r="L180" s="13"/>
-      <c r="M180" s="13"/>
-      <c r="N180" s="13"/>
+      <c r="G180" s="15"/>
+      <c r="H180" s="15"/>
+      <c r="I180" s="15"/>
+      <c r="J180" s="15"/>
+      <c r="K180" s="15"/>
+      <c r="L180" s="15"/>
+      <c r="M180" s="15"/>
+      <c r="N180" s="15"/>
     </row>
     <row r="181" spans="1:14">
-      <c r="A181" s="15"/>
-      <c r="B181" s="16"/>
-      <c r="C181" s="12" t="s">
+      <c r="A181" s="13"/>
+      <c r="B181" s="14"/>
+      <c r="C181" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D181" s="9">
+      <c r="D181" s="6">
         <v>0.125</v>
       </c>
-      <c r="E181" s="9">
+      <c r="E181" s="6">
         <v>0.27083333333333331</v>
       </c>
-      <c r="F181" s="13" t="s">
+      <c r="F181" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="G181" s="13"/>
-      <c r="H181" s="13"/>
-      <c r="I181" s="13"/>
-      <c r="J181" s="13"/>
-      <c r="K181" s="13"/>
-      <c r="L181" s="13"/>
-      <c r="M181" s="13"/>
-      <c r="N181" s="13"/>
+      <c r="G181" s="15"/>
+      <c r="H181" s="15"/>
+      <c r="I181" s="15"/>
+      <c r="J181" s="15"/>
+      <c r="K181" s="15"/>
+      <c r="L181" s="15"/>
+      <c r="M181" s="15"/>
+      <c r="N181" s="15"/>
+    </row>
+    <row r="184" spans="1:14">
+      <c r="A184" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B184" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C184" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D184" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E184" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F184" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G184" s="19"/>
+      <c r="H184" s="19"/>
+      <c r="I184" s="19"/>
+      <c r="J184" s="19"/>
+      <c r="K184" s="19"/>
+      <c r="L184" s="19"/>
+      <c r="M184" s="19"/>
+      <c r="N184" s="19"/>
+    </row>
+    <row r="185" spans="1:14">
+      <c r="A185" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B185" s="14">
+        <v>44981</v>
+      </c>
+      <c r="C185" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D185" s="6">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E185" s="6">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="F185" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G185" s="15"/>
+      <c r="H185" s="15"/>
+      <c r="I185" s="15"/>
+      <c r="J185" s="15"/>
+      <c r="K185" s="15"/>
+      <c r="L185" s="15"/>
+      <c r="M185" s="15"/>
+      <c r="N185" s="15"/>
+    </row>
+    <row r="186" spans="1:14">
+      <c r="A186" s="13"/>
+      <c r="B186" s="14"/>
+      <c r="C186" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D186" s="6">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="E186" s="6">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F186" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G186" s="15"/>
+      <c r="H186" s="15"/>
+      <c r="I186" s="15"/>
+      <c r="J186" s="15"/>
+      <c r="K186" s="15"/>
+      <c r="L186" s="15"/>
+      <c r="M186" s="15"/>
+      <c r="N186" s="15"/>
+    </row>
+    <row r="187" spans="1:14">
+      <c r="A187" s="13"/>
+      <c r="B187" s="14"/>
+      <c r="C187" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D187" s="6">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E187" s="6">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="F187" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G187" s="15"/>
+      <c r="H187" s="15"/>
+      <c r="I187" s="15"/>
+      <c r="J187" s="15"/>
+      <c r="K187" s="15"/>
+      <c r="L187" s="15"/>
+      <c r="M187" s="15"/>
+      <c r="N187" s="15"/>
+    </row>
+    <row r="188" spans="1:14">
+      <c r="A188" s="13"/>
+      <c r="B188" s="14"/>
+      <c r="C188" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D188" s="6">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="E188" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F188" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G188" s="15"/>
+      <c r="H188" s="15"/>
+      <c r="I188" s="15"/>
+      <c r="J188" s="15"/>
+      <c r="K188" s="15"/>
+      <c r="L188" s="15"/>
+      <c r="M188" s="15"/>
+      <c r="N188" s="15"/>
+    </row>
+    <row r="189" spans="1:14">
+      <c r="A189" s="13"/>
+      <c r="B189" s="14"/>
+      <c r="C189" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D189" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E189" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F189" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G189" s="15"/>
+      <c r="H189" s="15"/>
+      <c r="I189" s="15"/>
+      <c r="J189" s="15"/>
+      <c r="K189" s="15"/>
+      <c r="L189" s="15"/>
+      <c r="M189" s="15"/>
+      <c r="N189" s="15"/>
+    </row>
+    <row r="190" spans="1:14">
+      <c r="A190" s="13"/>
+      <c r="B190" s="14"/>
+      <c r="C190" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D190" s="6">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E190" s="6">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="F190" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G190" s="15"/>
+      <c r="H190" s="15"/>
+      <c r="I190" s="15"/>
+      <c r="J190" s="15"/>
+      <c r="K190" s="15"/>
+      <c r="L190" s="15"/>
+      <c r="M190" s="15"/>
+      <c r="N190" s="15"/>
+    </row>
+    <row r="191" spans="1:14">
+      <c r="A191" s="13"/>
+      <c r="B191" s="14"/>
+      <c r="C191" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D191" s="6">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="E191" s="6">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="F191" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G191" s="15"/>
+      <c r="H191" s="15"/>
+      <c r="I191" s="15"/>
+      <c r="J191" s="15"/>
+      <c r="K191" s="15"/>
+      <c r="L191" s="15"/>
+      <c r="M191" s="15"/>
+      <c r="N191" s="15"/>
+    </row>
+    <row r="192" spans="1:14">
+      <c r="A192" s="13"/>
+      <c r="B192" s="14"/>
+      <c r="C192" s="9"/>
+      <c r="D192" s="6">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="E192" s="6">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="F192" s="15"/>
+      <c r="G192" s="15"/>
+      <c r="H192" s="15"/>
+      <c r="I192" s="15"/>
+      <c r="J192" s="15"/>
+      <c r="K192" s="15"/>
+      <c r="L192" s="15"/>
+      <c r="M192" s="15"/>
+      <c r="N192" s="15"/>
+    </row>
+    <row r="197" spans="1:14">
+      <c r="A197" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B197" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C197" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="D197" s="50"/>
+      <c r="E197" s="50"/>
+      <c r="F197" s="50"/>
+      <c r="G197" s="50"/>
+      <c r="H197" s="50"/>
+      <c r="I197" s="50"/>
+      <c r="J197" s="50"/>
+      <c r="K197" s="50"/>
+      <c r="L197" s="50"/>
+      <c r="M197" s="50"/>
+      <c r="N197" s="51"/>
+    </row>
+    <row r="198" spans="1:14">
+      <c r="A198" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B198" s="32">
+        <v>44982</v>
+      </c>
+      <c r="C198" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D198" s="21"/>
+      <c r="E198" s="21"/>
+      <c r="F198" s="21"/>
+      <c r="G198" s="21"/>
+      <c r="H198" s="21"/>
+      <c r="I198" s="21"/>
+      <c r="J198" s="21"/>
+      <c r="K198" s="21"/>
+      <c r="L198" s="21"/>
+      <c r="M198" s="21"/>
+      <c r="N198" s="22"/>
+    </row>
+    <row r="199" spans="1:14">
+      <c r="A199" s="30"/>
+      <c r="B199" s="33"/>
+      <c r="C199" s="23"/>
+      <c r="D199" s="24"/>
+      <c r="E199" s="24"/>
+      <c r="F199" s="24"/>
+      <c r="G199" s="24"/>
+      <c r="H199" s="24"/>
+      <c r="I199" s="24"/>
+      <c r="J199" s="24"/>
+      <c r="K199" s="24"/>
+      <c r="L199" s="24"/>
+      <c r="M199" s="24"/>
+      <c r="N199" s="25"/>
+    </row>
+    <row r="200" spans="1:14">
+      <c r="A200" s="31"/>
+      <c r="B200" s="34"/>
+      <c r="C200" s="26"/>
+      <c r="D200" s="27"/>
+      <c r="E200" s="27"/>
+      <c r="F200" s="27"/>
+      <c r="G200" s="27"/>
+      <c r="H200" s="27"/>
+      <c r="I200" s="27"/>
+      <c r="J200" s="27"/>
+      <c r="K200" s="27"/>
+      <c r="L200" s="27"/>
+      <c r="M200" s="27"/>
+      <c r="N200" s="28"/>
+    </row>
+    <row r="203" spans="1:14">
+      <c r="A203" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B203" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C203" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D203" s="36"/>
+      <c r="E203" s="36"/>
+      <c r="F203" s="36"/>
+      <c r="G203" s="36"/>
+      <c r="H203" s="36"/>
+      <c r="I203" s="36"/>
+      <c r="J203" s="36"/>
+      <c r="K203" s="36"/>
+      <c r="L203" s="36"/>
+      <c r="M203" s="36"/>
+      <c r="N203" s="37"/>
+    </row>
+    <row r="204" spans="1:14">
+      <c r="A204" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B204" s="32">
+        <v>44983</v>
+      </c>
+      <c r="C204" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D204" s="21"/>
+      <c r="E204" s="21"/>
+      <c r="F204" s="21"/>
+      <c r="G204" s="21"/>
+      <c r="H204" s="21"/>
+      <c r="I204" s="21"/>
+      <c r="J204" s="21"/>
+      <c r="K204" s="21"/>
+      <c r="L204" s="21"/>
+      <c r="M204" s="21"/>
+      <c r="N204" s="22"/>
+    </row>
+    <row r="205" spans="1:14">
+      <c r="A205" s="30"/>
+      <c r="B205" s="33"/>
+      <c r="C205" s="23"/>
+      <c r="D205" s="24"/>
+      <c r="E205" s="24"/>
+      <c r="F205" s="24"/>
+      <c r="G205" s="24"/>
+      <c r="H205" s="24"/>
+      <c r="I205" s="24"/>
+      <c r="J205" s="24"/>
+      <c r="K205" s="24"/>
+      <c r="L205" s="24"/>
+      <c r="M205" s="24"/>
+      <c r="N205" s="25"/>
+    </row>
+    <row r="206" spans="1:14">
+      <c r="A206" s="31"/>
+      <c r="B206" s="34"/>
+      <c r="C206" s="26"/>
+      <c r="D206" s="27"/>
+      <c r="E206" s="27"/>
+      <c r="F206" s="27"/>
+      <c r="G206" s="27"/>
+      <c r="H206" s="27"/>
+      <c r="I206" s="27"/>
+      <c r="J206" s="27"/>
+      <c r="K206" s="27"/>
+      <c r="L206" s="27"/>
+      <c r="M206" s="27"/>
+      <c r="N206" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="61">
-    <mergeCell ref="F156:N156"/>
-    <mergeCell ref="A157:A160"/>
-    <mergeCell ref="B157:B160"/>
-    <mergeCell ref="F157:N157"/>
-    <mergeCell ref="F158:N158"/>
-    <mergeCell ref="F159:N159"/>
-    <mergeCell ref="F160:N160"/>
-    <mergeCell ref="F163:N163"/>
-    <mergeCell ref="A164:A166"/>
-    <mergeCell ref="B164:B166"/>
-    <mergeCell ref="F164:N164"/>
-    <mergeCell ref="F165:N165"/>
-    <mergeCell ref="F166:N166"/>
-    <mergeCell ref="C145:N147"/>
-    <mergeCell ref="A151:A153"/>
-    <mergeCell ref="B151:B153"/>
-    <mergeCell ref="C151:N153"/>
-    <mergeCell ref="C90:N92"/>
-    <mergeCell ref="A90:A92"/>
-    <mergeCell ref="B90:B92"/>
-    <mergeCell ref="A145:A147"/>
-    <mergeCell ref="B145:B147"/>
-    <mergeCell ref="C89:N89"/>
-    <mergeCell ref="A84:A86"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="C84:N86"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A67:A73"/>
-    <mergeCell ref="C77:N77"/>
-    <mergeCell ref="A78:A80"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="C78:N80"/>
-    <mergeCell ref="C83:N83"/>
-    <mergeCell ref="C35:N35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C36:N38"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:N32"/>
-    <mergeCell ref="C29:N29"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A10:A16"/>
-    <mergeCell ref="A21:A26"/>
+  <mergeCells count="82">
+    <mergeCell ref="A204:A206"/>
+    <mergeCell ref="B204:B206"/>
+    <mergeCell ref="C204:N206"/>
+    <mergeCell ref="F191:N191"/>
+    <mergeCell ref="B185:B192"/>
+    <mergeCell ref="A185:A192"/>
+    <mergeCell ref="F192:N192"/>
+    <mergeCell ref="C197:N197"/>
+    <mergeCell ref="A198:A200"/>
+    <mergeCell ref="B198:B200"/>
+    <mergeCell ref="C198:N200"/>
+    <mergeCell ref="C203:N203"/>
+    <mergeCell ref="F184:N184"/>
+    <mergeCell ref="F185:N185"/>
+    <mergeCell ref="F186:N186"/>
+    <mergeCell ref="F187:N187"/>
+    <mergeCell ref="F188:N188"/>
+    <mergeCell ref="F189:N189"/>
+    <mergeCell ref="F190:N190"/>
     <mergeCell ref="F181:N181"/>
     <mergeCell ref="F179:N179"/>
     <mergeCell ref="F180:N180"/>
@@ -2592,15 +2980,63 @@
     <mergeCell ref="F178:N178"/>
     <mergeCell ref="A176:A181"/>
     <mergeCell ref="B176:B181"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:N32"/>
+    <mergeCell ref="C29:N29"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="C35:N35"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:N38"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="C89:N89"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="C84:N86"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A67:A73"/>
+    <mergeCell ref="C77:N77"/>
+    <mergeCell ref="A78:A80"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="C78:N80"/>
+    <mergeCell ref="C83:N83"/>
+    <mergeCell ref="C145:N147"/>
+    <mergeCell ref="A151:A153"/>
+    <mergeCell ref="B151:B153"/>
+    <mergeCell ref="C151:N153"/>
+    <mergeCell ref="C90:N92"/>
+    <mergeCell ref="A90:A92"/>
+    <mergeCell ref="B90:B92"/>
+    <mergeCell ref="A145:A147"/>
+    <mergeCell ref="B145:B147"/>
+    <mergeCell ref="C144:N144"/>
+    <mergeCell ref="C150:N150"/>
+    <mergeCell ref="F163:N163"/>
+    <mergeCell ref="A164:A166"/>
+    <mergeCell ref="B164:B166"/>
+    <mergeCell ref="F164:N164"/>
+    <mergeCell ref="F165:N165"/>
+    <mergeCell ref="F166:N166"/>
+    <mergeCell ref="F156:N156"/>
+    <mergeCell ref="A157:A160"/>
+    <mergeCell ref="B157:B160"/>
+    <mergeCell ref="F157:N157"/>
+    <mergeCell ref="F158:N158"/>
+    <mergeCell ref="F159:N159"/>
+    <mergeCell ref="F160:N160"/>
   </mergeCells>
-  <conditionalFormatting sqref="B90:C90">
-    <cfRule type="timePeriod" dxfId="1" priority="2" timePeriod="lastMonth">
+  <conditionalFormatting sqref="B90:C90 B151:C151">
+    <cfRule type="timePeriod" dxfId="1" priority="3" timePeriod="lastMonth">
       <formula>AND(MONTH(B90)=MONTH(TODAY())-1,OR(YEAR(B90)=YEAR(TODAY()),AND(MONTH(B90)=1,YEAR(B90)=YEAR(TODAY())-1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B151:C151">
+  <conditionalFormatting sqref="B204:C204">
     <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="lastMonth">
-      <formula>AND(MONTH(B151)=MONTH(TODAY())-1,OR(YEAR(B151)=YEAR(TODAY()),AND(MONTH(B151)=1,YEAR(B151)=YEAR(TODAY())-1)))</formula>
+      <formula>AND(MONTH(B204)=MONTH(TODAY())-1,OR(YEAR(B204)=YEAR(TODAY()),AND(MONTH(B204)=1,YEAR(B204)=YEAR(TODAY())-1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
24 feb 2023 update
24 feb 2023 update
</commit_message>
<xml_diff>
--- a/feb/feb2023.xlsx
+++ b/feb/feb2023.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="48">
   <si>
     <t>Day</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>user module automatically fill username and Password and raise the PR</t>
+  </si>
+  <si>
+    <t>WBX-4079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go through the issue N Try to solve the issue </t>
   </si>
 </sst>
 </file>
@@ -449,21 +455,120 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="6" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -472,105 +577,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="7" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="6" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -581,17 +587,7 @@
     <cellStyle name="Bad" xfId="5" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1341,7 +1337,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1352,7 +1348,7 @@
   <dimension ref="A1:N206"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="T195" sqref="T195"/>
+      <selection activeCell="M194" sqref="M194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1368,18 +1364,18 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="48"/>
+      <c r="A3" s="36"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="48"/>
+      <c r="A4" s="36"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="48"/>
+      <c r="A5" s="36"/>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="1" t="s">
@@ -1387,27 +1383,27 @@
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="36" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="48"/>
+      <c r="A11" s="36"/>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="48"/>
+      <c r="A12" s="36"/>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="48"/>
+      <c r="A13" s="36"/>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="48"/>
+      <c r="A14" s="36"/>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="48"/>
+      <c r="A15" s="36"/>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="48"/>
+      <c r="A16" s="36"/>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
@@ -1415,24 +1411,24 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="48" t="s">
+      <c r="A21" s="36" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="48"/>
+      <c r="A22" s="36"/>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="48"/>
+      <c r="A23" s="36"/>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="48"/>
+      <c r="A24" s="36"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="48"/>
+      <c r="A25" s="36"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="48"/>
+      <c r="A26" s="36"/>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="2"/>
@@ -1444,74 +1440,74 @@
       <c r="B29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="36"/>
-      <c r="N29" s="37"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="34"/>
     </row>
     <row r="30" spans="1:14">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="32">
+      <c r="B30" s="14">
         <v>44961</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="22"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="19"/>
     </row>
     <row r="31" spans="1:14">
-      <c r="A31" s="30"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="25"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="22"/>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="31"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
-      <c r="L32" s="27"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="28"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="25"/>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="3" t="s">
@@ -1520,74 +1516,74 @@
       <c r="B35" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="35" t="s">
+      <c r="C35" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="36"/>
-      <c r="N35" s="37"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="33"/>
+      <c r="M35" s="33"/>
+      <c r="N35" s="34"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="32">
+      <c r="B36" s="14">
         <v>44962</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="21"/>
-      <c r="L36" s="21"/>
-      <c r="M36" s="21"/>
-      <c r="N36" s="22"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="19"/>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="30"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="24"/>
-      <c r="L37" s="24"/>
-      <c r="M37" s="24"/>
-      <c r="N37" s="25"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="22"/>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="31"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="27"/>
-      <c r="L38" s="27"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="28"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="24"/>
+      <c r="L38" s="24"/>
+      <c r="M38" s="24"/>
+      <c r="N38" s="25"/>
     </row>
     <row r="41" spans="1:14">
       <c r="A41" s="3" t="s">
@@ -1595,18 +1591,18 @@
       </c>
     </row>
     <row r="42" spans="1:14">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="28" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:14">
-      <c r="A43" s="13"/>
+      <c r="A43" s="28"/>
     </row>
     <row r="44" spans="1:14">
-      <c r="A44" s="13"/>
+      <c r="A44" s="28"/>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="13"/>
+      <c r="A45" s="28"/>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="3" t="s">
@@ -1614,15 +1610,15 @@
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="28" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="13"/>
+      <c r="A51" s="28"/>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="13"/>
+      <c r="A52" s="28"/>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="5" t="s">
@@ -1630,27 +1626,27 @@
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="38" t="s">
+      <c r="A56" s="37" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="38"/>
+      <c r="A57" s="37"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="38"/>
+      <c r="A58" s="37"/>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="38"/>
+      <c r="A59" s="37"/>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="38"/>
+      <c r="A60" s="37"/>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="38"/>
+      <c r="A61" s="37"/>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="38"/>
+      <c r="A62" s="37"/>
     </row>
     <row r="66" spans="1:14">
       <c r="A66" s="5" t="s">
@@ -1658,27 +1654,27 @@
       </c>
     </row>
     <row r="67" spans="1:14">
-      <c r="A67" s="38" t="s">
+      <c r="A67" s="37" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:14">
-      <c r="A68" s="38"/>
+      <c r="A68" s="37"/>
     </row>
     <row r="69" spans="1:14">
-      <c r="A69" s="38"/>
+      <c r="A69" s="37"/>
     </row>
     <row r="70" spans="1:14">
-      <c r="A70" s="38"/>
+      <c r="A70" s="37"/>
     </row>
     <row r="71" spans="1:14">
-      <c r="A71" s="38"/>
+      <c r="A71" s="37"/>
     </row>
     <row r="72" spans="1:14">
-      <c r="A72" s="38"/>
+      <c r="A72" s="37"/>
     </row>
     <row r="73" spans="1:14">
-      <c r="A73" s="38"/>
+      <c r="A73" s="37"/>
     </row>
     <row r="77" spans="1:14">
       <c r="A77" s="3" t="s">
@@ -1687,74 +1683,74 @@
       <c r="B77" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C77" s="35" t="s">
+      <c r="C77" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D77" s="36"/>
-      <c r="E77" s="36"/>
-      <c r="F77" s="36"/>
-      <c r="G77" s="36"/>
-      <c r="H77" s="36"/>
-      <c r="I77" s="36"/>
-      <c r="J77" s="36"/>
-      <c r="K77" s="36"/>
-      <c r="L77" s="36"/>
-      <c r="M77" s="36"/>
-      <c r="N77" s="37"/>
+      <c r="D77" s="33"/>
+      <c r="E77" s="33"/>
+      <c r="F77" s="33"/>
+      <c r="G77" s="33"/>
+      <c r="H77" s="33"/>
+      <c r="I77" s="33"/>
+      <c r="J77" s="33"/>
+      <c r="K77" s="33"/>
+      <c r="L77" s="33"/>
+      <c r="M77" s="33"/>
+      <c r="N77" s="34"/>
     </row>
     <row r="78" spans="1:14">
-      <c r="A78" s="29" t="s">
+      <c r="A78" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B78" s="32">
+      <c r="B78" s="14">
         <v>44967</v>
       </c>
-      <c r="C78" s="39" t="s">
+      <c r="C78" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="D78" s="40"/>
-      <c r="E78" s="40"/>
-      <c r="F78" s="40"/>
-      <c r="G78" s="40"/>
-      <c r="H78" s="40"/>
-      <c r="I78" s="40"/>
-      <c r="J78" s="40"/>
-      <c r="K78" s="40"/>
-      <c r="L78" s="40"/>
-      <c r="M78" s="40"/>
-      <c r="N78" s="41"/>
+      <c r="D78" s="39"/>
+      <c r="E78" s="39"/>
+      <c r="F78" s="39"/>
+      <c r="G78" s="39"/>
+      <c r="H78" s="39"/>
+      <c r="I78" s="39"/>
+      <c r="J78" s="39"/>
+      <c r="K78" s="39"/>
+      <c r="L78" s="39"/>
+      <c r="M78" s="39"/>
+      <c r="N78" s="40"/>
     </row>
     <row r="79" spans="1:14">
-      <c r="A79" s="30"/>
-      <c r="B79" s="33"/>
-      <c r="C79" s="42"/>
-      <c r="D79" s="43"/>
-      <c r="E79" s="43"/>
-      <c r="F79" s="43"/>
-      <c r="G79" s="43"/>
-      <c r="H79" s="43"/>
-      <c r="I79" s="43"/>
-      <c r="J79" s="43"/>
-      <c r="K79" s="43"/>
-      <c r="L79" s="43"/>
-      <c r="M79" s="43"/>
-      <c r="N79" s="44"/>
+      <c r="A79" s="12"/>
+      <c r="B79" s="15"/>
+      <c r="C79" s="41"/>
+      <c r="D79" s="42"/>
+      <c r="E79" s="42"/>
+      <c r="F79" s="42"/>
+      <c r="G79" s="42"/>
+      <c r="H79" s="42"/>
+      <c r="I79" s="42"/>
+      <c r="J79" s="42"/>
+      <c r="K79" s="42"/>
+      <c r="L79" s="42"/>
+      <c r="M79" s="42"/>
+      <c r="N79" s="43"/>
     </row>
     <row r="80" spans="1:14">
-      <c r="A80" s="31"/>
-      <c r="B80" s="34"/>
-      <c r="C80" s="45"/>
-      <c r="D80" s="46"/>
-      <c r="E80" s="46"/>
-      <c r="F80" s="46"/>
-      <c r="G80" s="46"/>
-      <c r="H80" s="46"/>
-      <c r="I80" s="46"/>
-      <c r="J80" s="46"/>
-      <c r="K80" s="46"/>
-      <c r="L80" s="46"/>
-      <c r="M80" s="46"/>
-      <c r="N80" s="47"/>
+      <c r="A80" s="13"/>
+      <c r="B80" s="16"/>
+      <c r="C80" s="44"/>
+      <c r="D80" s="45"/>
+      <c r="E80" s="45"/>
+      <c r="F80" s="45"/>
+      <c r="G80" s="45"/>
+      <c r="H80" s="45"/>
+      <c r="I80" s="45"/>
+      <c r="J80" s="45"/>
+      <c r="K80" s="45"/>
+      <c r="L80" s="45"/>
+      <c r="M80" s="45"/>
+      <c r="N80" s="46"/>
     </row>
     <row r="83" spans="1:14">
       <c r="A83" s="3" t="s">
@@ -1763,74 +1759,74 @@
       <c r="B83" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C83" s="35" t="s">
+      <c r="C83" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D83" s="36"/>
-      <c r="E83" s="36"/>
-      <c r="F83" s="36"/>
-      <c r="G83" s="36"/>
-      <c r="H83" s="36"/>
-      <c r="I83" s="36"/>
-      <c r="J83" s="36"/>
-      <c r="K83" s="36"/>
-      <c r="L83" s="36"/>
-      <c r="M83" s="36"/>
-      <c r="N83" s="37"/>
+      <c r="D83" s="33"/>
+      <c r="E83" s="33"/>
+      <c r="F83" s="33"/>
+      <c r="G83" s="33"/>
+      <c r="H83" s="33"/>
+      <c r="I83" s="33"/>
+      <c r="J83" s="33"/>
+      <c r="K83" s="33"/>
+      <c r="L83" s="33"/>
+      <c r="M83" s="33"/>
+      <c r="N83" s="34"/>
     </row>
     <row r="84" spans="1:14">
-      <c r="A84" s="29" t="s">
+      <c r="A84" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B84" s="32">
+      <c r="B84" s="14">
         <v>44968</v>
       </c>
-      <c r="C84" s="20" t="s">
+      <c r="C84" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D84" s="21"/>
-      <c r="E84" s="21"/>
-      <c r="F84" s="21"/>
-      <c r="G84" s="21"/>
-      <c r="H84" s="21"/>
-      <c r="I84" s="21"/>
-      <c r="J84" s="21"/>
-      <c r="K84" s="21"/>
-      <c r="L84" s="21"/>
-      <c r="M84" s="21"/>
-      <c r="N84" s="22"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
+      <c r="I84" s="18"/>
+      <c r="J84" s="18"/>
+      <c r="K84" s="18"/>
+      <c r="L84" s="18"/>
+      <c r="M84" s="18"/>
+      <c r="N84" s="19"/>
     </row>
     <row r="85" spans="1:14">
-      <c r="A85" s="30"/>
-      <c r="B85" s="33"/>
-      <c r="C85" s="23"/>
-      <c r="D85" s="24"/>
-      <c r="E85" s="24"/>
-      <c r="F85" s="24"/>
-      <c r="G85" s="24"/>
-      <c r="H85" s="24"/>
-      <c r="I85" s="24"/>
-      <c r="J85" s="24"/>
-      <c r="K85" s="24"/>
-      <c r="L85" s="24"/>
-      <c r="M85" s="24"/>
-      <c r="N85" s="25"/>
+      <c r="A85" s="12"/>
+      <c r="B85" s="15"/>
+      <c r="C85" s="20"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="21"/>
+      <c r="H85" s="21"/>
+      <c r="I85" s="21"/>
+      <c r="J85" s="21"/>
+      <c r="K85" s="21"/>
+      <c r="L85" s="21"/>
+      <c r="M85" s="21"/>
+      <c r="N85" s="22"/>
     </row>
     <row r="86" spans="1:14">
-      <c r="A86" s="31"/>
-      <c r="B86" s="34"/>
-      <c r="C86" s="26"/>
-      <c r="D86" s="27"/>
-      <c r="E86" s="27"/>
-      <c r="F86" s="27"/>
-      <c r="G86" s="27"/>
-      <c r="H86" s="27"/>
-      <c r="I86" s="27"/>
-      <c r="J86" s="27"/>
-      <c r="K86" s="27"/>
-      <c r="L86" s="27"/>
-      <c r="M86" s="27"/>
-      <c r="N86" s="28"/>
+      <c r="A86" s="13"/>
+      <c r="B86" s="16"/>
+      <c r="C86" s="23"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="24"/>
+      <c r="F86" s="24"/>
+      <c r="G86" s="24"/>
+      <c r="H86" s="24"/>
+      <c r="I86" s="24"/>
+      <c r="J86" s="24"/>
+      <c r="K86" s="24"/>
+      <c r="L86" s="24"/>
+      <c r="M86" s="24"/>
+      <c r="N86" s="25"/>
     </row>
     <row r="89" spans="1:14">
       <c r="A89" s="3" t="s">
@@ -1839,74 +1835,74 @@
       <c r="B89" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C89" s="35" t="s">
+      <c r="C89" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D89" s="36"/>
-      <c r="E89" s="36"/>
-      <c r="F89" s="36"/>
-      <c r="G89" s="36"/>
-      <c r="H89" s="36"/>
-      <c r="I89" s="36"/>
-      <c r="J89" s="36"/>
-      <c r="K89" s="36"/>
-      <c r="L89" s="36"/>
-      <c r="M89" s="36"/>
-      <c r="N89" s="37"/>
+      <c r="D89" s="33"/>
+      <c r="E89" s="33"/>
+      <c r="F89" s="33"/>
+      <c r="G89" s="33"/>
+      <c r="H89" s="33"/>
+      <c r="I89" s="33"/>
+      <c r="J89" s="33"/>
+      <c r="K89" s="33"/>
+      <c r="L89" s="33"/>
+      <c r="M89" s="33"/>
+      <c r="N89" s="34"/>
     </row>
     <row r="90" spans="1:14">
-      <c r="A90" s="29" t="s">
+      <c r="A90" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B90" s="32">
+      <c r="B90" s="14">
         <v>44969</v>
       </c>
-      <c r="C90" s="20" t="s">
+      <c r="C90" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D90" s="21"/>
-      <c r="E90" s="21"/>
-      <c r="F90" s="21"/>
-      <c r="G90" s="21"/>
-      <c r="H90" s="21"/>
-      <c r="I90" s="21"/>
-      <c r="J90" s="21"/>
-      <c r="K90" s="21"/>
-      <c r="L90" s="21"/>
-      <c r="M90" s="21"/>
-      <c r="N90" s="22"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="18"/>
+      <c r="G90" s="18"/>
+      <c r="H90" s="18"/>
+      <c r="I90" s="18"/>
+      <c r="J90" s="18"/>
+      <c r="K90" s="18"/>
+      <c r="L90" s="18"/>
+      <c r="M90" s="18"/>
+      <c r="N90" s="19"/>
     </row>
     <row r="91" spans="1:14">
-      <c r="A91" s="30"/>
-      <c r="B91" s="33"/>
-      <c r="C91" s="23"/>
-      <c r="D91" s="24"/>
-      <c r="E91" s="24"/>
-      <c r="F91" s="24"/>
-      <c r="G91" s="24"/>
-      <c r="H91" s="24"/>
-      <c r="I91" s="24"/>
-      <c r="J91" s="24"/>
-      <c r="K91" s="24"/>
-      <c r="L91" s="24"/>
-      <c r="M91" s="24"/>
-      <c r="N91" s="25"/>
+      <c r="A91" s="12"/>
+      <c r="B91" s="15"/>
+      <c r="C91" s="20"/>
+      <c r="D91" s="21"/>
+      <c r="E91" s="21"/>
+      <c r="F91" s="21"/>
+      <c r="G91" s="21"/>
+      <c r="H91" s="21"/>
+      <c r="I91" s="21"/>
+      <c r="J91" s="21"/>
+      <c r="K91" s="21"/>
+      <c r="L91" s="21"/>
+      <c r="M91" s="21"/>
+      <c r="N91" s="22"/>
     </row>
     <row r="92" spans="1:14">
-      <c r="A92" s="31"/>
-      <c r="B92" s="34"/>
-      <c r="C92" s="26"/>
-      <c r="D92" s="27"/>
-      <c r="E92" s="27"/>
-      <c r="F92" s="27"/>
-      <c r="G92" s="27"/>
-      <c r="H92" s="27"/>
-      <c r="I92" s="27"/>
-      <c r="J92" s="27"/>
-      <c r="K92" s="27"/>
-      <c r="L92" s="27"/>
-      <c r="M92" s="27"/>
-      <c r="N92" s="28"/>
+      <c r="A92" s="13"/>
+      <c r="B92" s="16"/>
+      <c r="C92" s="23"/>
+      <c r="D92" s="24"/>
+      <c r="E92" s="24"/>
+      <c r="F92" s="24"/>
+      <c r="G92" s="24"/>
+      <c r="H92" s="24"/>
+      <c r="I92" s="24"/>
+      <c r="J92" s="24"/>
+      <c r="K92" s="24"/>
+      <c r="L92" s="24"/>
+      <c r="M92" s="24"/>
+      <c r="N92" s="25"/>
     </row>
     <row r="144" spans="1:14">
       <c r="A144" s="3" t="s">
@@ -1915,74 +1911,74 @@
       <c r="B144" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C144" s="49" t="s">
+      <c r="C144" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D144" s="50"/>
-      <c r="E144" s="50"/>
-      <c r="F144" s="50"/>
-      <c r="G144" s="50"/>
-      <c r="H144" s="50"/>
-      <c r="I144" s="50"/>
-      <c r="J144" s="50"/>
-      <c r="K144" s="50"/>
-      <c r="L144" s="50"/>
-      <c r="M144" s="50"/>
-      <c r="N144" s="51"/>
+      <c r="D144" s="30"/>
+      <c r="E144" s="30"/>
+      <c r="F144" s="30"/>
+      <c r="G144" s="30"/>
+      <c r="H144" s="30"/>
+      <c r="I144" s="30"/>
+      <c r="J144" s="30"/>
+      <c r="K144" s="30"/>
+      <c r="L144" s="30"/>
+      <c r="M144" s="30"/>
+      <c r="N144" s="31"/>
     </row>
     <row r="145" spans="1:14">
-      <c r="A145" s="29" t="s">
+      <c r="A145" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B145" s="32">
+      <c r="B145" s="14">
         <v>44975</v>
       </c>
-      <c r="C145" s="20" t="s">
+      <c r="C145" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D145" s="21"/>
-      <c r="E145" s="21"/>
-      <c r="F145" s="21"/>
-      <c r="G145" s="21"/>
-      <c r="H145" s="21"/>
-      <c r="I145" s="21"/>
-      <c r="J145" s="21"/>
-      <c r="K145" s="21"/>
-      <c r="L145" s="21"/>
-      <c r="M145" s="21"/>
-      <c r="N145" s="22"/>
+      <c r="D145" s="18"/>
+      <c r="E145" s="18"/>
+      <c r="F145" s="18"/>
+      <c r="G145" s="18"/>
+      <c r="H145" s="18"/>
+      <c r="I145" s="18"/>
+      <c r="J145" s="18"/>
+      <c r="K145" s="18"/>
+      <c r="L145" s="18"/>
+      <c r="M145" s="18"/>
+      <c r="N145" s="19"/>
     </row>
     <row r="146" spans="1:14">
-      <c r="A146" s="30"/>
-      <c r="B146" s="33"/>
-      <c r="C146" s="23"/>
-      <c r="D146" s="24"/>
-      <c r="E146" s="24"/>
-      <c r="F146" s="24"/>
-      <c r="G146" s="24"/>
-      <c r="H146" s="24"/>
-      <c r="I146" s="24"/>
-      <c r="J146" s="24"/>
-      <c r="K146" s="24"/>
-      <c r="L146" s="24"/>
-      <c r="M146" s="24"/>
-      <c r="N146" s="25"/>
+      <c r="A146" s="12"/>
+      <c r="B146" s="15"/>
+      <c r="C146" s="20"/>
+      <c r="D146" s="21"/>
+      <c r="E146" s="21"/>
+      <c r="F146" s="21"/>
+      <c r="G146" s="21"/>
+      <c r="H146" s="21"/>
+      <c r="I146" s="21"/>
+      <c r="J146" s="21"/>
+      <c r="K146" s="21"/>
+      <c r="L146" s="21"/>
+      <c r="M146" s="21"/>
+      <c r="N146" s="22"/>
     </row>
     <row r="147" spans="1:14">
-      <c r="A147" s="31"/>
-      <c r="B147" s="34"/>
-      <c r="C147" s="26"/>
-      <c r="D147" s="27"/>
-      <c r="E147" s="27"/>
-      <c r="F147" s="27"/>
-      <c r="G147" s="27"/>
-      <c r="H147" s="27"/>
-      <c r="I147" s="27"/>
-      <c r="J147" s="27"/>
-      <c r="K147" s="27"/>
-      <c r="L147" s="27"/>
-      <c r="M147" s="27"/>
-      <c r="N147" s="28"/>
+      <c r="A147" s="13"/>
+      <c r="B147" s="16"/>
+      <c r="C147" s="23"/>
+      <c r="D147" s="24"/>
+      <c r="E147" s="24"/>
+      <c r="F147" s="24"/>
+      <c r="G147" s="24"/>
+      <c r="H147" s="24"/>
+      <c r="I147" s="24"/>
+      <c r="J147" s="24"/>
+      <c r="K147" s="24"/>
+      <c r="L147" s="24"/>
+      <c r="M147" s="24"/>
+      <c r="N147" s="25"/>
     </row>
     <row r="150" spans="1:14">
       <c r="A150" s="3" t="s">
@@ -1991,74 +1987,74 @@
       <c r="B150" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C150" s="35" t="s">
+      <c r="C150" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D150" s="36"/>
-      <c r="E150" s="36"/>
-      <c r="F150" s="36"/>
-      <c r="G150" s="36"/>
-      <c r="H150" s="36"/>
-      <c r="I150" s="36"/>
-      <c r="J150" s="36"/>
-      <c r="K150" s="36"/>
-      <c r="L150" s="36"/>
-      <c r="M150" s="36"/>
-      <c r="N150" s="37"/>
+      <c r="D150" s="33"/>
+      <c r="E150" s="33"/>
+      <c r="F150" s="33"/>
+      <c r="G150" s="33"/>
+      <c r="H150" s="33"/>
+      <c r="I150" s="33"/>
+      <c r="J150" s="33"/>
+      <c r="K150" s="33"/>
+      <c r="L150" s="33"/>
+      <c r="M150" s="33"/>
+      <c r="N150" s="34"/>
     </row>
     <row r="151" spans="1:14">
-      <c r="A151" s="29" t="s">
+      <c r="A151" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B151" s="32">
+      <c r="B151" s="14">
         <v>44976</v>
       </c>
-      <c r="C151" s="20" t="s">
+      <c r="C151" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D151" s="21"/>
-      <c r="E151" s="21"/>
-      <c r="F151" s="21"/>
-      <c r="G151" s="21"/>
-      <c r="H151" s="21"/>
-      <c r="I151" s="21"/>
-      <c r="J151" s="21"/>
-      <c r="K151" s="21"/>
-      <c r="L151" s="21"/>
-      <c r="M151" s="21"/>
-      <c r="N151" s="22"/>
+      <c r="D151" s="18"/>
+      <c r="E151" s="18"/>
+      <c r="F151" s="18"/>
+      <c r="G151" s="18"/>
+      <c r="H151" s="18"/>
+      <c r="I151" s="18"/>
+      <c r="J151" s="18"/>
+      <c r="K151" s="18"/>
+      <c r="L151" s="18"/>
+      <c r="M151" s="18"/>
+      <c r="N151" s="19"/>
     </row>
     <row r="152" spans="1:14">
-      <c r="A152" s="30"/>
-      <c r="B152" s="33"/>
-      <c r="C152" s="23"/>
-      <c r="D152" s="24"/>
-      <c r="E152" s="24"/>
-      <c r="F152" s="24"/>
-      <c r="G152" s="24"/>
-      <c r="H152" s="24"/>
-      <c r="I152" s="24"/>
-      <c r="J152" s="24"/>
-      <c r="K152" s="24"/>
-      <c r="L152" s="24"/>
-      <c r="M152" s="24"/>
-      <c r="N152" s="25"/>
+      <c r="A152" s="12"/>
+      <c r="B152" s="15"/>
+      <c r="C152" s="20"/>
+      <c r="D152" s="21"/>
+      <c r="E152" s="21"/>
+      <c r="F152" s="21"/>
+      <c r="G152" s="21"/>
+      <c r="H152" s="21"/>
+      <c r="I152" s="21"/>
+      <c r="J152" s="21"/>
+      <c r="K152" s="21"/>
+      <c r="L152" s="21"/>
+      <c r="M152" s="21"/>
+      <c r="N152" s="22"/>
     </row>
     <row r="153" spans="1:14">
-      <c r="A153" s="31"/>
-      <c r="B153" s="34"/>
-      <c r="C153" s="26"/>
-      <c r="D153" s="27"/>
-      <c r="E153" s="27"/>
-      <c r="F153" s="27"/>
-      <c r="G153" s="27"/>
-      <c r="H153" s="27"/>
-      <c r="I153" s="27"/>
-      <c r="J153" s="27"/>
-      <c r="K153" s="27"/>
-      <c r="L153" s="27"/>
-      <c r="M153" s="27"/>
-      <c r="N153" s="28"/>
+      <c r="A153" s="13"/>
+      <c r="B153" s="16"/>
+      <c r="C153" s="23"/>
+      <c r="D153" s="24"/>
+      <c r="E153" s="24"/>
+      <c r="F153" s="24"/>
+      <c r="G153" s="24"/>
+      <c r="H153" s="24"/>
+      <c r="I153" s="24"/>
+      <c r="J153" s="24"/>
+      <c r="K153" s="24"/>
+      <c r="L153" s="24"/>
+      <c r="M153" s="24"/>
+      <c r="N153" s="25"/>
     </row>
     <row r="156" spans="1:14">
       <c r="A156" s="3" t="s">
@@ -2076,23 +2072,23 @@
       <c r="E156" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F156" s="11" t="s">
+      <c r="F156" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="G156" s="12"/>
-      <c r="H156" s="12"/>
-      <c r="I156" s="12"/>
-      <c r="J156" s="12"/>
-      <c r="K156" s="12"/>
-      <c r="L156" s="12"/>
-      <c r="M156" s="12"/>
-      <c r="N156" s="12"/>
+      <c r="G156" s="48"/>
+      <c r="H156" s="48"/>
+      <c r="I156" s="48"/>
+      <c r="J156" s="48"/>
+      <c r="K156" s="48"/>
+      <c r="L156" s="48"/>
+      <c r="M156" s="48"/>
+      <c r="N156" s="48"/>
     </row>
     <row r="157" spans="1:14">
-      <c r="A157" s="13" t="s">
+      <c r="A157" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B157" s="14">
+      <c r="B157" s="27">
         <v>44977</v>
       </c>
       <c r="C157" s="6" t="s">
@@ -2104,21 +2100,21 @@
       <c r="E157" s="6">
         <v>0.40277777777777773</v>
       </c>
-      <c r="F157" s="15" t="s">
+      <c r="F157" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G157" s="15"/>
-      <c r="H157" s="15"/>
-      <c r="I157" s="15"/>
-      <c r="J157" s="15"/>
-      <c r="K157" s="15"/>
-      <c r="L157" s="15"/>
-      <c r="M157" s="15"/>
-      <c r="N157" s="15"/>
+      <c r="G157" s="26"/>
+      <c r="H157" s="26"/>
+      <c r="I157" s="26"/>
+      <c r="J157" s="26"/>
+      <c r="K157" s="26"/>
+      <c r="L157" s="26"/>
+      <c r="M157" s="26"/>
+      <c r="N157" s="26"/>
     </row>
     <row r="158" spans="1:14">
-      <c r="A158" s="13"/>
-      <c r="B158" s="14"/>
+      <c r="A158" s="28"/>
+      <c r="B158" s="27"/>
       <c r="C158" s="6" t="s">
         <v>19</v>
       </c>
@@ -2128,21 +2124,21 @@
       <c r="E158" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F158" s="15" t="s">
+      <c r="F158" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="G158" s="15"/>
-      <c r="H158" s="15"/>
-      <c r="I158" s="15"/>
-      <c r="J158" s="15"/>
-      <c r="K158" s="15"/>
-      <c r="L158" s="15"/>
-      <c r="M158" s="15"/>
-      <c r="N158" s="15"/>
+      <c r="G158" s="26"/>
+      <c r="H158" s="26"/>
+      <c r="I158" s="26"/>
+      <c r="J158" s="26"/>
+      <c r="K158" s="26"/>
+      <c r="L158" s="26"/>
+      <c r="M158" s="26"/>
+      <c r="N158" s="26"/>
     </row>
     <row r="159" spans="1:14">
-      <c r="A159" s="13"/>
-      <c r="B159" s="14"/>
+      <c r="A159" s="28"/>
+      <c r="B159" s="27"/>
       <c r="C159" s="7" t="s">
         <v>21</v>
       </c>
@@ -2152,21 +2148,21 @@
       <c r="E159" s="6">
         <v>0.22916666666666666</v>
       </c>
-      <c r="F159" s="16" t="s">
+      <c r="F159" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="G159" s="17"/>
-      <c r="H159" s="17"/>
-      <c r="I159" s="17"/>
-      <c r="J159" s="17"/>
-      <c r="K159" s="17"/>
-      <c r="L159" s="17"/>
-      <c r="M159" s="17"/>
-      <c r="N159" s="18"/>
+      <c r="G159" s="50"/>
+      <c r="H159" s="50"/>
+      <c r="I159" s="50"/>
+      <c r="J159" s="50"/>
+      <c r="K159" s="50"/>
+      <c r="L159" s="50"/>
+      <c r="M159" s="50"/>
+      <c r="N159" s="51"/>
     </row>
     <row r="160" spans="1:14">
-      <c r="A160" s="13"/>
-      <c r="B160" s="14"/>
+      <c r="A160" s="28"/>
+      <c r="B160" s="27"/>
       <c r="C160" s="7" t="s">
         <v>23</v>
       </c>
@@ -2176,17 +2172,17 @@
       <c r="E160" s="6">
         <v>0.27083333333333331</v>
       </c>
-      <c r="F160" s="15" t="s">
+      <c r="F160" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="G160" s="15"/>
-      <c r="H160" s="15"/>
-      <c r="I160" s="15"/>
-      <c r="J160" s="15"/>
-      <c r="K160" s="15"/>
-      <c r="L160" s="15"/>
-      <c r="M160" s="15"/>
-      <c r="N160" s="15"/>
+      <c r="G160" s="26"/>
+      <c r="H160" s="26"/>
+      <c r="I160" s="26"/>
+      <c r="J160" s="26"/>
+      <c r="K160" s="26"/>
+      <c r="L160" s="26"/>
+      <c r="M160" s="26"/>
+      <c r="N160" s="26"/>
     </row>
     <row r="163" spans="1:14">
       <c r="A163" s="3" t="s">
@@ -2204,23 +2200,23 @@
       <c r="E163" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F163" s="19" t="s">
+      <c r="F163" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="G163" s="19"/>
-      <c r="H163" s="19"/>
-      <c r="I163" s="19"/>
-      <c r="J163" s="19"/>
-      <c r="K163" s="19"/>
-      <c r="L163" s="19"/>
-      <c r="M163" s="19"/>
-      <c r="N163" s="19"/>
+      <c r="G163" s="35"/>
+      <c r="H163" s="35"/>
+      <c r="I163" s="35"/>
+      <c r="J163" s="35"/>
+      <c r="K163" s="35"/>
+      <c r="L163" s="35"/>
+      <c r="M163" s="35"/>
+      <c r="N163" s="35"/>
     </row>
     <row r="164" spans="1:14">
-      <c r="A164" s="13" t="s">
+      <c r="A164" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B164" s="14">
+      <c r="B164" s="27">
         <v>44978</v>
       </c>
       <c r="C164" s="6" t="s">
@@ -2232,21 +2228,21 @@
       <c r="E164" s="6">
         <v>0.40277777777777773</v>
       </c>
-      <c r="F164" s="15" t="s">
+      <c r="F164" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G164" s="15"/>
-      <c r="H164" s="15"/>
-      <c r="I164" s="15"/>
-      <c r="J164" s="15"/>
-      <c r="K164" s="15"/>
-      <c r="L164" s="15"/>
-      <c r="M164" s="15"/>
-      <c r="N164" s="15"/>
+      <c r="G164" s="26"/>
+      <c r="H164" s="26"/>
+      <c r="I164" s="26"/>
+      <c r="J164" s="26"/>
+      <c r="K164" s="26"/>
+      <c r="L164" s="26"/>
+      <c r="M164" s="26"/>
+      <c r="N164" s="26"/>
     </row>
     <row r="165" spans="1:14">
-      <c r="A165" s="13"/>
-      <c r="B165" s="14"/>
+      <c r="A165" s="28"/>
+      <c r="B165" s="27"/>
       <c r="C165" s="7" t="s">
         <v>12</v>
       </c>
@@ -2256,21 +2252,21 @@
       <c r="E165" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F165" s="15" t="s">
+      <c r="F165" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="G165" s="15"/>
-      <c r="H165" s="15"/>
-      <c r="I165" s="15"/>
-      <c r="J165" s="15"/>
-      <c r="K165" s="15"/>
-      <c r="L165" s="15"/>
-      <c r="M165" s="15"/>
-      <c r="N165" s="15"/>
+      <c r="G165" s="26"/>
+      <c r="H165" s="26"/>
+      <c r="I165" s="26"/>
+      <c r="J165" s="26"/>
+      <c r="K165" s="26"/>
+      <c r="L165" s="26"/>
+      <c r="M165" s="26"/>
+      <c r="N165" s="26"/>
     </row>
     <row r="166" spans="1:14">
-      <c r="A166" s="13"/>
-      <c r="B166" s="14"/>
+      <c r="A166" s="28"/>
+      <c r="B166" s="27"/>
       <c r="C166" s="7" t="s">
         <v>12</v>
       </c>
@@ -2280,17 +2276,17 @@
       <c r="E166" s="6">
         <v>0.27083333333333331</v>
       </c>
-      <c r="F166" s="15" t="s">
+      <c r="F166" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="G166" s="15"/>
-      <c r="H166" s="15"/>
-      <c r="I166" s="15"/>
-      <c r="J166" s="15"/>
-      <c r="K166" s="15"/>
-      <c r="L166" s="15"/>
-      <c r="M166" s="15"/>
-      <c r="N166" s="15"/>
+      <c r="G166" s="26"/>
+      <c r="H166" s="26"/>
+      <c r="I166" s="26"/>
+      <c r="J166" s="26"/>
+      <c r="K166" s="26"/>
+      <c r="L166" s="26"/>
+      <c r="M166" s="26"/>
+      <c r="N166" s="26"/>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="4" t="s">
@@ -2308,23 +2304,23 @@
       <c r="E169" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F169" s="19" t="s">
+      <c r="F169" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="G169" s="19"/>
-      <c r="H169" s="19"/>
-      <c r="I169" s="19"/>
-      <c r="J169" s="19"/>
-      <c r="K169" s="19"/>
-      <c r="L169" s="19"/>
-      <c r="M169" s="19"/>
-      <c r="N169" s="19"/>
+      <c r="G169" s="35"/>
+      <c r="H169" s="35"/>
+      <c r="I169" s="35"/>
+      <c r="J169" s="35"/>
+      <c r="K169" s="35"/>
+      <c r="L169" s="35"/>
+      <c r="M169" s="35"/>
+      <c r="N169" s="35"/>
     </row>
     <row r="170" spans="1:14">
-      <c r="A170" s="13" t="s">
+      <c r="A170" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B170" s="14">
+      <c r="B170" s="27">
         <v>44979</v>
       </c>
       <c r="C170" s="6" t="s">
@@ -2336,21 +2332,21 @@
       <c r="E170" s="6">
         <v>0.40277777777777773</v>
       </c>
-      <c r="F170" s="15" t="s">
+      <c r="F170" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G170" s="15"/>
-      <c r="H170" s="15"/>
-      <c r="I170" s="15"/>
-      <c r="J170" s="15"/>
-      <c r="K170" s="15"/>
-      <c r="L170" s="15"/>
-      <c r="M170" s="15"/>
-      <c r="N170" s="15"/>
+      <c r="G170" s="26"/>
+      <c r="H170" s="26"/>
+      <c r="I170" s="26"/>
+      <c r="J170" s="26"/>
+      <c r="K170" s="26"/>
+      <c r="L170" s="26"/>
+      <c r="M170" s="26"/>
+      <c r="N170" s="26"/>
     </row>
     <row r="171" spans="1:14">
-      <c r="A171" s="13"/>
-      <c r="B171" s="14"/>
+      <c r="A171" s="28"/>
+      <c r="B171" s="27"/>
       <c r="C171" s="7" t="s">
         <v>21</v>
       </c>
@@ -2360,21 +2356,21 @@
       <c r="E171" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F171" s="15" t="s">
+      <c r="F171" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="G171" s="15"/>
-      <c r="H171" s="15"/>
-      <c r="I171" s="15"/>
-      <c r="J171" s="15"/>
-      <c r="K171" s="15"/>
-      <c r="L171" s="15"/>
-      <c r="M171" s="15"/>
-      <c r="N171" s="15"/>
+      <c r="G171" s="26"/>
+      <c r="H171" s="26"/>
+      <c r="I171" s="26"/>
+      <c r="J171" s="26"/>
+      <c r="K171" s="26"/>
+      <c r="L171" s="26"/>
+      <c r="M171" s="26"/>
+      <c r="N171" s="26"/>
     </row>
     <row r="172" spans="1:14">
-      <c r="A172" s="13"/>
-      <c r="B172" s="14"/>
+      <c r="A172" s="28"/>
+      <c r="B172" s="27"/>
       <c r="C172" s="7" t="s">
         <v>12</v>
       </c>
@@ -2384,17 +2380,17 @@
       <c r="E172" s="6">
         <v>0.27083333333333331</v>
       </c>
-      <c r="F172" s="15" t="s">
+      <c r="F172" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="G172" s="15"/>
-      <c r="H172" s="15"/>
-      <c r="I172" s="15"/>
-      <c r="J172" s="15"/>
-      <c r="K172" s="15"/>
-      <c r="L172" s="15"/>
-      <c r="M172" s="15"/>
-      <c r="N172" s="15"/>
+      <c r="G172" s="26"/>
+      <c r="H172" s="26"/>
+      <c r="I172" s="26"/>
+      <c r="J172" s="26"/>
+      <c r="K172" s="26"/>
+      <c r="L172" s="26"/>
+      <c r="M172" s="26"/>
+      <c r="N172" s="26"/>
     </row>
     <row r="175" spans="1:14">
       <c r="A175" s="8" t="s">
@@ -2412,23 +2408,23 @@
       <c r="E175" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F175" s="19" t="s">
+      <c r="F175" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="G175" s="19"/>
-      <c r="H175" s="19"/>
-      <c r="I175" s="19"/>
-      <c r="J175" s="19"/>
-      <c r="K175" s="19"/>
-      <c r="L175" s="19"/>
-      <c r="M175" s="19"/>
-      <c r="N175" s="19"/>
+      <c r="G175" s="35"/>
+      <c r="H175" s="35"/>
+      <c r="I175" s="35"/>
+      <c r="J175" s="35"/>
+      <c r="K175" s="35"/>
+      <c r="L175" s="35"/>
+      <c r="M175" s="35"/>
+      <c r="N175" s="35"/>
     </row>
     <row r="176" spans="1:14">
-      <c r="A176" s="13" t="s">
+      <c r="A176" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B176" s="14">
+      <c r="B176" s="27">
         <v>44980</v>
       </c>
       <c r="C176" s="9" t="s">
@@ -2440,21 +2436,21 @@
       <c r="E176" s="6">
         <v>0.40277777777777773</v>
       </c>
-      <c r="F176" s="15" t="s">
+      <c r="F176" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G176" s="15"/>
-      <c r="H176" s="15"/>
-      <c r="I176" s="15"/>
-      <c r="J176" s="15"/>
-      <c r="K176" s="15"/>
-      <c r="L176" s="15"/>
-      <c r="M176" s="15"/>
-      <c r="N176" s="15"/>
+      <c r="G176" s="26"/>
+      <c r="H176" s="26"/>
+      <c r="I176" s="26"/>
+      <c r="J176" s="26"/>
+      <c r="K176" s="26"/>
+      <c r="L176" s="26"/>
+      <c r="M176" s="26"/>
+      <c r="N176" s="26"/>
     </row>
     <row r="177" spans="1:14">
-      <c r="A177" s="13"/>
-      <c r="B177" s="14"/>
+      <c r="A177" s="28"/>
+      <c r="B177" s="27"/>
       <c r="C177" s="9" t="s">
         <v>23</v>
       </c>
@@ -2464,21 +2460,21 @@
       <c r="E177" s="6">
         <v>0.48125000000000001</v>
       </c>
-      <c r="F177" s="15" t="s">
+      <c r="F177" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="G177" s="15"/>
-      <c r="H177" s="15"/>
-      <c r="I177" s="15"/>
-      <c r="J177" s="15"/>
-      <c r="K177" s="15"/>
-      <c r="L177" s="15"/>
-      <c r="M177" s="15"/>
-      <c r="N177" s="15"/>
+      <c r="G177" s="26"/>
+      <c r="H177" s="26"/>
+      <c r="I177" s="26"/>
+      <c r="J177" s="26"/>
+      <c r="K177" s="26"/>
+      <c r="L177" s="26"/>
+      <c r="M177" s="26"/>
+      <c r="N177" s="26"/>
     </row>
     <row r="178" spans="1:14">
-      <c r="A178" s="13"/>
-      <c r="B178" s="14"/>
+      <c r="A178" s="28"/>
+      <c r="B178" s="27"/>
       <c r="C178" s="9" t="s">
         <v>10</v>
       </c>
@@ -2488,21 +2484,21 @@
       <c r="E178" s="6">
         <v>0.5</v>
       </c>
-      <c r="F178" s="15" t="s">
+      <c r="F178" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="G178" s="15"/>
-      <c r="H178" s="15"/>
-      <c r="I178" s="15"/>
-      <c r="J178" s="15"/>
-      <c r="K178" s="15"/>
-      <c r="L178" s="15"/>
-      <c r="M178" s="15"/>
-      <c r="N178" s="15"/>
+      <c r="G178" s="26"/>
+      <c r="H178" s="26"/>
+      <c r="I178" s="26"/>
+      <c r="J178" s="26"/>
+      <c r="K178" s="26"/>
+      <c r="L178" s="26"/>
+      <c r="M178" s="26"/>
+      <c r="N178" s="26"/>
     </row>
     <row r="179" spans="1:14">
-      <c r="A179" s="13"/>
-      <c r="B179" s="14"/>
+      <c r="A179" s="28"/>
+      <c r="B179" s="27"/>
       <c r="C179" s="9" t="s">
         <v>28</v>
       </c>
@@ -2512,21 +2508,21 @@
       <c r="E179" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F179" s="15" t="s">
+      <c r="F179" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="G179" s="15"/>
-      <c r="H179" s="15"/>
-      <c r="I179" s="15"/>
-      <c r="J179" s="15"/>
-      <c r="K179" s="15"/>
-      <c r="L179" s="15"/>
-      <c r="M179" s="15"/>
-      <c r="N179" s="15"/>
+      <c r="G179" s="26"/>
+      <c r="H179" s="26"/>
+      <c r="I179" s="26"/>
+      <c r="J179" s="26"/>
+      <c r="K179" s="26"/>
+      <c r="L179" s="26"/>
+      <c r="M179" s="26"/>
+      <c r="N179" s="26"/>
     </row>
     <row r="180" spans="1:14">
-      <c r="A180" s="13"/>
-      <c r="B180" s="14"/>
+      <c r="A180" s="28"/>
+      <c r="B180" s="27"/>
       <c r="C180" s="9" t="s">
         <v>29</v>
       </c>
@@ -2536,21 +2532,21 @@
       <c r="E180" s="6">
         <v>0.125</v>
       </c>
-      <c r="F180" s="15" t="s">
+      <c r="F180" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="G180" s="15"/>
-      <c r="H180" s="15"/>
-      <c r="I180" s="15"/>
-      <c r="J180" s="15"/>
-      <c r="K180" s="15"/>
-      <c r="L180" s="15"/>
-      <c r="M180" s="15"/>
-      <c r="N180" s="15"/>
+      <c r="G180" s="26"/>
+      <c r="H180" s="26"/>
+      <c r="I180" s="26"/>
+      <c r="J180" s="26"/>
+      <c r="K180" s="26"/>
+      <c r="L180" s="26"/>
+      <c r="M180" s="26"/>
+      <c r="N180" s="26"/>
     </row>
     <row r="181" spans="1:14">
-      <c r="A181" s="13"/>
-      <c r="B181" s="14"/>
+      <c r="A181" s="28"/>
+      <c r="B181" s="27"/>
       <c r="C181" s="9" t="s">
         <v>33</v>
       </c>
@@ -2560,17 +2556,17 @@
       <c r="E181" s="6">
         <v>0.27083333333333331</v>
       </c>
-      <c r="F181" s="15" t="s">
+      <c r="F181" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="G181" s="15"/>
-      <c r="H181" s="15"/>
-      <c r="I181" s="15"/>
-      <c r="J181" s="15"/>
-      <c r="K181" s="15"/>
-      <c r="L181" s="15"/>
-      <c r="M181" s="15"/>
-      <c r="N181" s="15"/>
+      <c r="G181" s="26"/>
+      <c r="H181" s="26"/>
+      <c r="I181" s="26"/>
+      <c r="J181" s="26"/>
+      <c r="K181" s="26"/>
+      <c r="L181" s="26"/>
+      <c r="M181" s="26"/>
+      <c r="N181" s="26"/>
     </row>
     <row r="184" spans="1:14">
       <c r="A184" s="10" t="s">
@@ -2588,23 +2584,23 @@
       <c r="E184" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F184" s="19" t="s">
+      <c r="F184" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="G184" s="19"/>
-      <c r="H184" s="19"/>
-      <c r="I184" s="19"/>
-      <c r="J184" s="19"/>
-      <c r="K184" s="19"/>
-      <c r="L184" s="19"/>
-      <c r="M184" s="19"/>
-      <c r="N184" s="19"/>
+      <c r="G184" s="35"/>
+      <c r="H184" s="35"/>
+      <c r="I184" s="35"/>
+      <c r="J184" s="35"/>
+      <c r="K184" s="35"/>
+      <c r="L184" s="35"/>
+      <c r="M184" s="35"/>
+      <c r="N184" s="35"/>
     </row>
     <row r="185" spans="1:14">
-      <c r="A185" s="13" t="s">
+      <c r="A185" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B185" s="14">
+      <c r="B185" s="27">
         <v>44981</v>
       </c>
       <c r="C185" s="9" t="s">
@@ -2616,21 +2612,21 @@
       <c r="E185" s="6">
         <v>0.40277777777777773</v>
       </c>
-      <c r="F185" s="15" t="s">
+      <c r="F185" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G185" s="15"/>
-      <c r="H185" s="15"/>
-      <c r="I185" s="15"/>
-      <c r="J185" s="15"/>
-      <c r="K185" s="15"/>
-      <c r="L185" s="15"/>
-      <c r="M185" s="15"/>
-      <c r="N185" s="15"/>
+      <c r="G185" s="26"/>
+      <c r="H185" s="26"/>
+      <c r="I185" s="26"/>
+      <c r="J185" s="26"/>
+      <c r="K185" s="26"/>
+      <c r="L185" s="26"/>
+      <c r="M185" s="26"/>
+      <c r="N185" s="26"/>
     </row>
     <row r="186" spans="1:14">
-      <c r="A186" s="13"/>
-      <c r="B186" s="14"/>
+      <c r="A186" s="28"/>
+      <c r="B186" s="27"/>
       <c r="C186" s="9" t="s">
         <v>33</v>
       </c>
@@ -2640,21 +2636,21 @@
       <c r="E186" s="6">
         <v>0.45833333333333331</v>
       </c>
-      <c r="F186" s="15" t="s">
+      <c r="F186" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="G186" s="15"/>
-      <c r="H186" s="15"/>
-      <c r="I186" s="15"/>
-      <c r="J186" s="15"/>
-      <c r="K186" s="15"/>
-      <c r="L186" s="15"/>
-      <c r="M186" s="15"/>
-      <c r="N186" s="15"/>
+      <c r="G186" s="26"/>
+      <c r="H186" s="26"/>
+      <c r="I186" s="26"/>
+      <c r="J186" s="26"/>
+      <c r="K186" s="26"/>
+      <c r="L186" s="26"/>
+      <c r="M186" s="26"/>
+      <c r="N186" s="26"/>
     </row>
     <row r="187" spans="1:14">
-      <c r="A187" s="13"/>
-      <c r="B187" s="14"/>
+      <c r="A187" s="28"/>
+      <c r="B187" s="27"/>
       <c r="C187" s="9" t="s">
         <v>29</v>
       </c>
@@ -2664,21 +2660,21 @@
       <c r="E187" s="6">
         <v>0.46527777777777773</v>
       </c>
-      <c r="F187" s="15" t="s">
+      <c r="F187" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="G187" s="15"/>
-      <c r="H187" s="15"/>
-      <c r="I187" s="15"/>
-      <c r="J187" s="15"/>
-      <c r="K187" s="15"/>
-      <c r="L187" s="15"/>
-      <c r="M187" s="15"/>
-      <c r="N187" s="15"/>
+      <c r="G187" s="26"/>
+      <c r="H187" s="26"/>
+      <c r="I187" s="26"/>
+      <c r="J187" s="26"/>
+      <c r="K187" s="26"/>
+      <c r="L187" s="26"/>
+      <c r="M187" s="26"/>
+      <c r="N187" s="26"/>
     </row>
     <row r="188" spans="1:14">
-      <c r="A188" s="13"/>
-      <c r="B188" s="14"/>
+      <c r="A188" s="28"/>
+      <c r="B188" s="27"/>
       <c r="C188" s="9" t="s">
         <v>38</v>
       </c>
@@ -2688,21 +2684,21 @@
       <c r="E188" s="6">
         <v>0.47916666666666669</v>
       </c>
-      <c r="F188" s="15" t="s">
+      <c r="F188" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="G188" s="15"/>
-      <c r="H188" s="15"/>
-      <c r="I188" s="15"/>
-      <c r="J188" s="15"/>
-      <c r="K188" s="15"/>
-      <c r="L188" s="15"/>
-      <c r="M188" s="15"/>
-      <c r="N188" s="15"/>
+      <c r="G188" s="26"/>
+      <c r="H188" s="26"/>
+      <c r="I188" s="26"/>
+      <c r="J188" s="26"/>
+      <c r="K188" s="26"/>
+      <c r="L188" s="26"/>
+      <c r="M188" s="26"/>
+      <c r="N188" s="26"/>
     </row>
     <row r="189" spans="1:14">
-      <c r="A189" s="13"/>
-      <c r="B189" s="14"/>
+      <c r="A189" s="28"/>
+      <c r="B189" s="27"/>
       <c r="C189" s="9" t="s">
         <v>40</v>
       </c>
@@ -2712,21 +2708,21 @@
       <c r="E189" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F189" s="15" t="s">
+      <c r="F189" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="G189" s="15"/>
-      <c r="H189" s="15"/>
-      <c r="I189" s="15"/>
-      <c r="J189" s="15"/>
-      <c r="K189" s="15"/>
-      <c r="L189" s="15"/>
-      <c r="M189" s="15"/>
-      <c r="N189" s="15"/>
+      <c r="G189" s="26"/>
+      <c r="H189" s="26"/>
+      <c r="I189" s="26"/>
+      <c r="J189" s="26"/>
+      <c r="K189" s="26"/>
+      <c r="L189" s="26"/>
+      <c r="M189" s="26"/>
+      <c r="N189" s="26"/>
     </row>
     <row r="190" spans="1:14">
-      <c r="A190" s="13"/>
-      <c r="B190" s="14"/>
+      <c r="A190" s="28"/>
+      <c r="B190" s="27"/>
       <c r="C190" s="9" t="s">
         <v>42</v>
       </c>
@@ -2736,21 +2732,21 @@
       <c r="E190" s="6">
         <v>0.10416666666666667</v>
       </c>
-      <c r="F190" s="15" t="s">
+      <c r="F190" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="G190" s="15"/>
-      <c r="H190" s="15"/>
-      <c r="I190" s="15"/>
-      <c r="J190" s="15"/>
-      <c r="K190" s="15"/>
-      <c r="L190" s="15"/>
-      <c r="M190" s="15"/>
-      <c r="N190" s="15"/>
+      <c r="G190" s="26"/>
+      <c r="H190" s="26"/>
+      <c r="I190" s="26"/>
+      <c r="J190" s="26"/>
+      <c r="K190" s="26"/>
+      <c r="L190" s="26"/>
+      <c r="M190" s="26"/>
+      <c r="N190" s="26"/>
     </row>
     <row r="191" spans="1:14">
-      <c r="A191" s="13"/>
-      <c r="B191" s="14"/>
+      <c r="A191" s="28"/>
+      <c r="B191" s="27"/>
       <c r="C191" s="9" t="s">
         <v>44</v>
       </c>
@@ -2760,37 +2756,41 @@
       <c r="E191" s="6">
         <v>0.22916666666666666</v>
       </c>
-      <c r="F191" s="15" t="s">
+      <c r="F191" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G191" s="15"/>
-      <c r="H191" s="15"/>
-      <c r="I191" s="15"/>
-      <c r="J191" s="15"/>
-      <c r="K191" s="15"/>
-      <c r="L191" s="15"/>
-      <c r="M191" s="15"/>
-      <c r="N191" s="15"/>
+      <c r="G191" s="26"/>
+      <c r="H191" s="26"/>
+      <c r="I191" s="26"/>
+      <c r="J191" s="26"/>
+      <c r="K191" s="26"/>
+      <c r="L191" s="26"/>
+      <c r="M191" s="26"/>
+      <c r="N191" s="26"/>
     </row>
     <row r="192" spans="1:14">
-      <c r="A192" s="13"/>
-      <c r="B192" s="14"/>
-      <c r="C192" s="9"/>
+      <c r="A192" s="28"/>
+      <c r="B192" s="27"/>
+      <c r="C192" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="D192" s="6">
         <v>0.22916666666666666</v>
       </c>
       <c r="E192" s="6">
         <v>0.27083333333333331</v>
       </c>
-      <c r="F192" s="15"/>
-      <c r="G192" s="15"/>
-      <c r="H192" s="15"/>
-      <c r="I192" s="15"/>
-      <c r="J192" s="15"/>
-      <c r="K192" s="15"/>
-      <c r="L192" s="15"/>
-      <c r="M192" s="15"/>
-      <c r="N192" s="15"/>
+      <c r="F192" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G192" s="26"/>
+      <c r="H192" s="26"/>
+      <c r="I192" s="26"/>
+      <c r="J192" s="26"/>
+      <c r="K192" s="26"/>
+      <c r="L192" s="26"/>
+      <c r="M192" s="26"/>
+      <c r="N192" s="26"/>
     </row>
     <row r="197" spans="1:14">
       <c r="A197" s="10" t="s">
@@ -2799,74 +2799,74 @@
       <c r="B197" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C197" s="49" t="s">
+      <c r="C197" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D197" s="50"/>
-      <c r="E197" s="50"/>
-      <c r="F197" s="50"/>
-      <c r="G197" s="50"/>
-      <c r="H197" s="50"/>
-      <c r="I197" s="50"/>
-      <c r="J197" s="50"/>
-      <c r="K197" s="50"/>
-      <c r="L197" s="50"/>
-      <c r="M197" s="50"/>
-      <c r="N197" s="51"/>
+      <c r="D197" s="30"/>
+      <c r="E197" s="30"/>
+      <c r="F197" s="30"/>
+      <c r="G197" s="30"/>
+      <c r="H197" s="30"/>
+      <c r="I197" s="30"/>
+      <c r="J197" s="30"/>
+      <c r="K197" s="30"/>
+      <c r="L197" s="30"/>
+      <c r="M197" s="30"/>
+      <c r="N197" s="31"/>
     </row>
     <row r="198" spans="1:14">
-      <c r="A198" s="29" t="s">
+      <c r="A198" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B198" s="32">
+      <c r="B198" s="14">
         <v>44982</v>
       </c>
-      <c r="C198" s="20" t="s">
+      <c r="C198" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D198" s="21"/>
-      <c r="E198" s="21"/>
-      <c r="F198" s="21"/>
-      <c r="G198" s="21"/>
-      <c r="H198" s="21"/>
-      <c r="I198" s="21"/>
-      <c r="J198" s="21"/>
-      <c r="K198" s="21"/>
-      <c r="L198" s="21"/>
-      <c r="M198" s="21"/>
-      <c r="N198" s="22"/>
+      <c r="D198" s="18"/>
+      <c r="E198" s="18"/>
+      <c r="F198" s="18"/>
+      <c r="G198" s="18"/>
+      <c r="H198" s="18"/>
+      <c r="I198" s="18"/>
+      <c r="J198" s="18"/>
+      <c r="K198" s="18"/>
+      <c r="L198" s="18"/>
+      <c r="M198" s="18"/>
+      <c r="N198" s="19"/>
     </row>
     <row r="199" spans="1:14">
-      <c r="A199" s="30"/>
-      <c r="B199" s="33"/>
-      <c r="C199" s="23"/>
-      <c r="D199" s="24"/>
-      <c r="E199" s="24"/>
-      <c r="F199" s="24"/>
-      <c r="G199" s="24"/>
-      <c r="H199" s="24"/>
-      <c r="I199" s="24"/>
-      <c r="J199" s="24"/>
-      <c r="K199" s="24"/>
-      <c r="L199" s="24"/>
-      <c r="M199" s="24"/>
-      <c r="N199" s="25"/>
+      <c r="A199" s="12"/>
+      <c r="B199" s="15"/>
+      <c r="C199" s="20"/>
+      <c r="D199" s="21"/>
+      <c r="E199" s="21"/>
+      <c r="F199" s="21"/>
+      <c r="G199" s="21"/>
+      <c r="H199" s="21"/>
+      <c r="I199" s="21"/>
+      <c r="J199" s="21"/>
+      <c r="K199" s="21"/>
+      <c r="L199" s="21"/>
+      <c r="M199" s="21"/>
+      <c r="N199" s="22"/>
     </row>
     <row r="200" spans="1:14">
-      <c r="A200" s="31"/>
-      <c r="B200" s="34"/>
-      <c r="C200" s="26"/>
-      <c r="D200" s="27"/>
-      <c r="E200" s="27"/>
-      <c r="F200" s="27"/>
-      <c r="G200" s="27"/>
-      <c r="H200" s="27"/>
-      <c r="I200" s="27"/>
-      <c r="J200" s="27"/>
-      <c r="K200" s="27"/>
-      <c r="L200" s="27"/>
-      <c r="M200" s="27"/>
-      <c r="N200" s="28"/>
+      <c r="A200" s="13"/>
+      <c r="B200" s="16"/>
+      <c r="C200" s="23"/>
+      <c r="D200" s="24"/>
+      <c r="E200" s="24"/>
+      <c r="F200" s="24"/>
+      <c r="G200" s="24"/>
+      <c r="H200" s="24"/>
+      <c r="I200" s="24"/>
+      <c r="J200" s="24"/>
+      <c r="K200" s="24"/>
+      <c r="L200" s="24"/>
+      <c r="M200" s="24"/>
+      <c r="N200" s="25"/>
     </row>
     <row r="203" spans="1:14">
       <c r="A203" s="10" t="s">
@@ -2875,96 +2875,125 @@
       <c r="B203" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C203" s="35" t="s">
+      <c r="C203" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D203" s="36"/>
-      <c r="E203" s="36"/>
-      <c r="F203" s="36"/>
-      <c r="G203" s="36"/>
-      <c r="H203" s="36"/>
-      <c r="I203" s="36"/>
-      <c r="J203" s="36"/>
-      <c r="K203" s="36"/>
-      <c r="L203" s="36"/>
-      <c r="M203" s="36"/>
-      <c r="N203" s="37"/>
+      <c r="D203" s="33"/>
+      <c r="E203" s="33"/>
+      <c r="F203" s="33"/>
+      <c r="G203" s="33"/>
+      <c r="H203" s="33"/>
+      <c r="I203" s="33"/>
+      <c r="J203" s="33"/>
+      <c r="K203" s="33"/>
+      <c r="L203" s="33"/>
+      <c r="M203" s="33"/>
+      <c r="N203" s="34"/>
     </row>
     <row r="204" spans="1:14">
-      <c r="A204" s="29" t="s">
+      <c r="A204" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B204" s="32">
+      <c r="B204" s="14">
         <v>44983</v>
       </c>
-      <c r="C204" s="20" t="s">
+      <c r="C204" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D204" s="21"/>
-      <c r="E204" s="21"/>
-      <c r="F204" s="21"/>
-      <c r="G204" s="21"/>
-      <c r="H204" s="21"/>
-      <c r="I204" s="21"/>
-      <c r="J204" s="21"/>
-      <c r="K204" s="21"/>
-      <c r="L204" s="21"/>
-      <c r="M204" s="21"/>
-      <c r="N204" s="22"/>
+      <c r="D204" s="18"/>
+      <c r="E204" s="18"/>
+      <c r="F204" s="18"/>
+      <c r="G204" s="18"/>
+      <c r="H204" s="18"/>
+      <c r="I204" s="18"/>
+      <c r="J204" s="18"/>
+      <c r="K204" s="18"/>
+      <c r="L204" s="18"/>
+      <c r="M204" s="18"/>
+      <c r="N204" s="19"/>
     </row>
     <row r="205" spans="1:14">
-      <c r="A205" s="30"/>
-      <c r="B205" s="33"/>
-      <c r="C205" s="23"/>
-      <c r="D205" s="24"/>
-      <c r="E205" s="24"/>
-      <c r="F205" s="24"/>
-      <c r="G205" s="24"/>
-      <c r="H205" s="24"/>
-      <c r="I205" s="24"/>
-      <c r="J205" s="24"/>
-      <c r="K205" s="24"/>
-      <c r="L205" s="24"/>
-      <c r="M205" s="24"/>
-      <c r="N205" s="25"/>
+      <c r="A205" s="12"/>
+      <c r="B205" s="15"/>
+      <c r="C205" s="20"/>
+      <c r="D205" s="21"/>
+      <c r="E205" s="21"/>
+      <c r="F205" s="21"/>
+      <c r="G205" s="21"/>
+      <c r="H205" s="21"/>
+      <c r="I205" s="21"/>
+      <c r="J205" s="21"/>
+      <c r="K205" s="21"/>
+      <c r="L205" s="21"/>
+      <c r="M205" s="21"/>
+      <c r="N205" s="22"/>
     </row>
     <row r="206" spans="1:14">
-      <c r="A206" s="31"/>
-      <c r="B206" s="34"/>
-      <c r="C206" s="26"/>
-      <c r="D206" s="27"/>
-      <c r="E206" s="27"/>
-      <c r="F206" s="27"/>
-      <c r="G206" s="27"/>
-      <c r="H206" s="27"/>
-      <c r="I206" s="27"/>
-      <c r="J206" s="27"/>
-      <c r="K206" s="27"/>
-      <c r="L206" s="27"/>
-      <c r="M206" s="27"/>
-      <c r="N206" s="28"/>
+      <c r="A206" s="13"/>
+      <c r="B206" s="16"/>
+      <c r="C206" s="23"/>
+      <c r="D206" s="24"/>
+      <c r="E206" s="24"/>
+      <c r="F206" s="24"/>
+      <c r="G206" s="24"/>
+      <c r="H206" s="24"/>
+      <c r="I206" s="24"/>
+      <c r="J206" s="24"/>
+      <c r="K206" s="24"/>
+      <c r="L206" s="24"/>
+      <c r="M206" s="24"/>
+      <c r="N206" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="A204:A206"/>
-    <mergeCell ref="B204:B206"/>
-    <mergeCell ref="C204:N206"/>
-    <mergeCell ref="F191:N191"/>
-    <mergeCell ref="B185:B192"/>
-    <mergeCell ref="A185:A192"/>
-    <mergeCell ref="F192:N192"/>
-    <mergeCell ref="C197:N197"/>
-    <mergeCell ref="A198:A200"/>
-    <mergeCell ref="B198:B200"/>
-    <mergeCell ref="C198:N200"/>
-    <mergeCell ref="C203:N203"/>
-    <mergeCell ref="F184:N184"/>
-    <mergeCell ref="F185:N185"/>
-    <mergeCell ref="F186:N186"/>
-    <mergeCell ref="F187:N187"/>
-    <mergeCell ref="F188:N188"/>
-    <mergeCell ref="F189:N189"/>
-    <mergeCell ref="F190:N190"/>
+    <mergeCell ref="F156:N156"/>
+    <mergeCell ref="A157:A160"/>
+    <mergeCell ref="B157:B160"/>
+    <mergeCell ref="F157:N157"/>
+    <mergeCell ref="F158:N158"/>
+    <mergeCell ref="F159:N159"/>
+    <mergeCell ref="F160:N160"/>
+    <mergeCell ref="F163:N163"/>
+    <mergeCell ref="A164:A166"/>
+    <mergeCell ref="B164:B166"/>
+    <mergeCell ref="F164:N164"/>
+    <mergeCell ref="F165:N165"/>
+    <mergeCell ref="F166:N166"/>
+    <mergeCell ref="C145:N147"/>
+    <mergeCell ref="A151:A153"/>
+    <mergeCell ref="B151:B153"/>
+    <mergeCell ref="C151:N153"/>
+    <mergeCell ref="C90:N92"/>
+    <mergeCell ref="A90:A92"/>
+    <mergeCell ref="B90:B92"/>
+    <mergeCell ref="A145:A147"/>
+    <mergeCell ref="B145:B147"/>
+    <mergeCell ref="C144:N144"/>
+    <mergeCell ref="C150:N150"/>
+    <mergeCell ref="C89:N89"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="C84:N86"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A56:A62"/>
+    <mergeCell ref="A67:A73"/>
+    <mergeCell ref="C77:N77"/>
+    <mergeCell ref="A78:A80"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="C78:N80"/>
+    <mergeCell ref="C83:N83"/>
+    <mergeCell ref="C35:N35"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:N38"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:N32"/>
+    <mergeCell ref="C29:N29"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="A21:A26"/>
     <mergeCell ref="F181:N181"/>
     <mergeCell ref="F179:N179"/>
     <mergeCell ref="F180:N180"/>
@@ -2980,54 +3009,25 @@
     <mergeCell ref="F178:N178"/>
     <mergeCell ref="A176:A181"/>
     <mergeCell ref="B176:B181"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:N32"/>
-    <mergeCell ref="C29:N29"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A10:A16"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="C35:N35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C36:N38"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="C89:N89"/>
-    <mergeCell ref="A84:A86"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="C84:N86"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A56:A62"/>
-    <mergeCell ref="A67:A73"/>
-    <mergeCell ref="C77:N77"/>
-    <mergeCell ref="A78:A80"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="C78:N80"/>
-    <mergeCell ref="C83:N83"/>
-    <mergeCell ref="C145:N147"/>
-    <mergeCell ref="A151:A153"/>
-    <mergeCell ref="B151:B153"/>
-    <mergeCell ref="C151:N153"/>
-    <mergeCell ref="C90:N92"/>
-    <mergeCell ref="A90:A92"/>
-    <mergeCell ref="B90:B92"/>
-    <mergeCell ref="A145:A147"/>
-    <mergeCell ref="B145:B147"/>
-    <mergeCell ref="C144:N144"/>
-    <mergeCell ref="C150:N150"/>
-    <mergeCell ref="F163:N163"/>
-    <mergeCell ref="A164:A166"/>
-    <mergeCell ref="B164:B166"/>
-    <mergeCell ref="F164:N164"/>
-    <mergeCell ref="F165:N165"/>
-    <mergeCell ref="F166:N166"/>
-    <mergeCell ref="F156:N156"/>
-    <mergeCell ref="A157:A160"/>
-    <mergeCell ref="B157:B160"/>
-    <mergeCell ref="F157:N157"/>
-    <mergeCell ref="F158:N158"/>
-    <mergeCell ref="F159:N159"/>
-    <mergeCell ref="F160:N160"/>
+    <mergeCell ref="F184:N184"/>
+    <mergeCell ref="F185:N185"/>
+    <mergeCell ref="F186:N186"/>
+    <mergeCell ref="F187:N187"/>
+    <mergeCell ref="F188:N188"/>
+    <mergeCell ref="A204:A206"/>
+    <mergeCell ref="B204:B206"/>
+    <mergeCell ref="C204:N206"/>
+    <mergeCell ref="F191:N191"/>
+    <mergeCell ref="B185:B192"/>
+    <mergeCell ref="A185:A192"/>
+    <mergeCell ref="F192:N192"/>
+    <mergeCell ref="C197:N197"/>
+    <mergeCell ref="A198:A200"/>
+    <mergeCell ref="B198:B200"/>
+    <mergeCell ref="C198:N200"/>
+    <mergeCell ref="C203:N203"/>
+    <mergeCell ref="F189:N189"/>
+    <mergeCell ref="F190:N190"/>
   </mergeCells>
   <conditionalFormatting sqref="B90:C90 B151:C151">
     <cfRule type="timePeriod" dxfId="1" priority="3" timePeriod="lastMonth">

</xml_diff>